<commit_message>
Uppdaterat TKB till PA47. Uppdaterat mappningsdokument för diagnos på motsvarande sätt. Mappningsdokument för Uppmärksamhetsinformation släpar fortfarande efter.
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/docs/Bilaga MIM_Mappningar_GetDiagnosis.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/docs/Bilaga MIM_Mappningar_GetDiagnosis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="12210" windowHeight="9945"/>
+    <workbookView xWindow="0" yWindow="240" windowWidth="12210" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="348">
   <si>
     <t>Meddelandestruktur</t>
   </si>
@@ -317,9 +317,6 @@
     <t>diagnos.händelsetidpunkt</t>
   </si>
   <si>
-    <t>diagnos.diagnostyp</t>
-  </si>
-  <si>
     <t>OBS</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t xml:space="preserve">Anger om information får delas till patient. Värdet sätts i sådant fall till true, i annat fall till false. </t>
   </si>
   <si>
-    <t>diagnos.relaterar til</t>
-  </si>
-  <si>
     <t>Transformering</t>
   </si>
   <si>
@@ -534,9 +528,6 @@
   </si>
   <si>
     <t>…section.code.displayName = Diagnos</t>
-  </si>
-  <si>
-    <t>Anges som "Huvuddiagnos", "Bidiagnos" eller "Kronisk diagnos".</t>
   </si>
   <si>
     <t>typeCode</t>
@@ -617,21 +608,9 @@
     <t>Id för patienten.</t>
   </si>
   <si>
-    <t>clinicalDocument.author.assignedAuthor.representedOrganization.id.extention = diagnosisHeader.author.careUnitHSAid</t>
-  </si>
-  <si>
-    <t>clinicalDocument.author.assignedAuthor.representedOrganization.addr = diagnosisHeader.author.careUnitHSAddress</t>
-  </si>
-  <si>
-    <t>clinicalDocument.author.assignedAuthor.representedOrganization.asOrganizationPartOf.wholeOrganization.id.extention = diagnosisHeader.author.careGiverHSAid</t>
-  </si>
-  <si>
     <t>clinicalDocument.legalAuthenticator.assignedEntity.representedOrganization.id.extention = diagnosisHeader.author.careUnitHSAid</t>
   </si>
   <si>
-    <t>clinicalDocument.author.assignedAuthor.assignedPerson.name = diagnosisHeader.author.authorName</t>
-  </si>
-  <si>
     <t>ClinicalDocument.custodian.assignedCustodian.representedCustodianOrganization.id.root = 1.2.752.129.2.1.4.1</t>
   </si>
   <si>
@@ -659,31 +638,16 @@
     <t>Klartext för kod som angivits i attributet diagnosisCode.</t>
   </si>
   <si>
-    <t>COMP</t>
-  </si>
-  <si>
-    <t>…section.entry.observation.entryRelationship.typeCode = COMP</t>
-  </si>
-  <si>
-    <t>entryrelationsship</t>
-  </si>
-  <si>
     <t>Kod som anger typ av tillgänglighet. Tillåtet värde är  310866003 för  Information till Patient (att information är tillgänglig till patient kan ha föregåtts av menprövning)</t>
   </si>
   <si>
     <t>clinicalDocument.authorization.consent.code = 310866003</t>
   </si>
   <si>
-    <t>ClinicalDocument.custodian.assignedCustodian.representedCustodianOrganization.id.extension = diagnosisHeader.author.careGiverHSAid</t>
-  </si>
-  <si>
     <t>ClinicalDocument.code.code = 439401001</t>
   </si>
   <si>
     <t>…section.code.code = 439401001</t>
-  </si>
-  <si>
-    <t>Koden (inom parenteser) för motsvarande diagnosisType: huvuddiagnos (8319008), bidiagnos (85097005) eller kronisk diagnos (90734009)</t>
   </si>
   <si>
     <t>informationsmängd.ägande vårdgivare-id</t>
@@ -735,9 +699,6 @@
     <t>HealthcareProfessionalType</t>
   </si>
   <si>
-    <t>healthcareProfessionalHSAid</t>
-  </si>
-  <si>
     <t>healthcareProfessionalRoleCode</t>
   </si>
   <si>
@@ -826,12 +787,6 @@
     <t>Information om den hälso- och sjukvårdsperson som skapat informationen i dokumentet, nedan kallad författare.</t>
   </si>
   <si>
-    <t>healthcareProfesssionalCareUnitHSAid</t>
-  </si>
-  <si>
-    <t>healthcareProfessionalCareGiverHSAid</t>
-  </si>
-  <si>
     <t>legalAuthenticatorName</t>
   </si>
   <si>
@@ -956,9 +911,6 @@
 Annars: clinicalDocument.author.assignedAuthor.code.codeSystem = 1.2.752.129.2.2.1.4</t>
   </si>
   <si>
-    <t>diagnosisId</t>
-  </si>
-  <si>
     <t>diagnosisTypeEnum</t>
   </si>
   <si>
@@ -1034,6 +986,87 @@
   <si>
     <t>originalText ska användas vid överföring av värden som kommer från lokala kodverk som ej är identifierade med OID eller när kod helt saknas. I sådana fall skall en beskrivande text anges i originalText.
 Om originalText anges kan inget av de övriga elementen anges. För NPÖ-kompabilitet bör inte detta fält användas.</t>
+  </si>
+  <si>
+    <t>clinicalDocument.author.assignedAuthor.assignedPerson.name = diagnosisHeader.accountableHealthcareProfessional.healthcareProfessionalName</t>
+  </si>
+  <si>
+    <t>clinicalDocument.author.assignedAuthor.representedOrganization.id.extention = diagnosisHeader.accountableHealthcareProfessional.careUnitHSAid</t>
+  </si>
+  <si>
+    <t>clinicalDocument.author.assignedAuthor.representedOrganization.addr = diagnosisHeader.accountableHealthcareProfessional.healthcareProfessionalOrgUnit.orgUnitAddress</t>
+  </si>
+  <si>
+    <t>clinicalDocument.author.assignedAuthor.representedOrganization.asOrganizationPartOf.wholeOrganization.id.extention = diagnosisHeader.accountableHealthcareProfessional.careGiverHSAid</t>
+  </si>
+  <si>
+    <t>ClinicalDocument.custodian.assignedCustodian.representedCustodianOrganization.id.extension = diagnosisHeader.accountableHealthcareProfessional.careUnitHSAid</t>
+  </si>
+  <si>
+    <t>healthcareProfesssionalCareUnitHSAId</t>
+  </si>
+  <si>
+    <t>healthcareProfessionalCareGiverHSAId</t>
+  </si>
+  <si>
+    <t>healthcareProfessionalHSAId</t>
+  </si>
+  <si>
+    <t>chronicDiagnosis</t>
+  </si>
+  <si>
+    <t>Sätts till true om diagnosen är kronisk, false om diagnosen inte är kronisk, och används inte om okänt.</t>
+  </si>
+  <si>
+    <t>Versionsangivelse av kodsystemet</t>
+  </si>
+  <si>
+    <t>diagnos.relaterar till</t>
+  </si>
+  <si>
+    <t>Anges som "Huvuddiagnos" eller "Bidiagnos".</t>
+  </si>
+  <si>
+    <t>REFR</t>
+  </si>
+  <si>
+    <t>Kronisk</t>
+  </si>
+  <si>
+    <t>diagnos.diagnostyp (i de fall diagnostyp = kronisk diagnos)</t>
+  </si>
+  <si>
+    <t>diagnos.diagnostyp (i de fall diagnostyp = huvuddiagnos eller bidiagnos)</t>
+  </si>
+  <si>
+    <t>entryRelationsship</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>Koden (inom parenteser) för motsvarande diagnosisType: huvuddiagnos (8319008), bidiagnos (85097005).</t>
+  </si>
+  <si>
+    <t>Denna …section.entry.observation.entryRelationship skapas bara om chronicDiagnosis är angiven</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.typeCode = REFR</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.observation.code.code = 90734009</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.observation.code.displayName = Kronisk</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.observation.code.codeSystem = 2.16.840.1.113883.6.96</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.observation.code.codeSystemName = SNOMED CT</t>
+  </si>
+  <si>
+    <t>…section.entry.observation.entryRelationship.observation.value = diagnosisBody.chronicDiagnosis</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1172,6 +1205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,7 +1265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1551,6 +1590,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1899,11 +1944,11 @@
   <sheetPr codeName="Blad2">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AO221"/>
+  <dimension ref="A1:AO222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG145" sqref="AG144:AG145"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2037,7 +2082,7 @@
       <c r="U3" s="119"/>
       <c r="V3" s="89"/>
       <c r="W3" s="71" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="X3" s="63"/>
       <c r="Y3" s="63"/>
@@ -2114,20 +2159,20 @@
       <c r="P5" s="15"/>
       <c r="Q5" s="110"/>
       <c r="R5" s="111" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="29" t="s">
         <v>32</v>
       </c>
       <c r="V5" s="91" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="W5" s="67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="X5" s="38"/>
       <c r="Y5" s="38"/>
@@ -2136,13 +2181,13 @@
       <c r="AB5" s="38"/>
       <c r="AC5" s="51"/>
       <c r="AD5" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AE5" s="64" t="s">
         <v>67</v>
       </c>
       <c r="AF5" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AG5" s="64" t="s">
         <v>32</v>
@@ -2214,7 +2259,7 @@
     </row>
     <row r="8" spans="1:41" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -2269,10 +2314,10 @@
       <c r="V9" s="75"/>
       <c r="W9" s="69"/>
       <c r="X9" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD9" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
@@ -2303,10 +2348,10 @@
       <c r="W10" s="69"/>
       <c r="X10" s="47"/>
       <c r="Y10" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD10" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2330,7 +2375,7 @@
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11" s="105" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S11" t="s">
         <v>1</v>
@@ -2373,7 +2418,7 @@
       </c>
       <c r="V12" s="78"/>
       <c r="W12" s="70" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:41" ht="25.5" x14ac:dyDescent="0.2">
@@ -2407,7 +2452,7 @@
       <c r="U13" s="7"/>
       <c r="V13" s="75"/>
       <c r="W13" s="70" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2431,14 +2476,14 @@
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14" s="105" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S14" t="s">
         <v>1</v>
       </c>
       <c r="T14" s="17"/>
       <c r="U14" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="V14" s="72"/>
       <c r="W14" s="70"/>
@@ -2472,27 +2517,27 @@
         <v>56</v>
       </c>
       <c r="U15" s="117" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="V15" s="73" t="s">
         <v>81</v>
       </c>
       <c r="W15" s="70" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG15" s="45" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:41" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2528,7 +2573,7 @@
       </c>
       <c r="V16" s="104"/>
       <c r="W16" s="70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z16" s="3"/>
     </row>
@@ -2594,7 +2639,7 @@
       </c>
       <c r="V18" s="72"/>
       <c r="W18" s="70" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="Z18" s="3"/>
       <c r="AE18" s="43"/>
@@ -2626,14 +2671,14 @@
         <v>1</v>
       </c>
       <c r="T19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="U19" s="32" t="s">
         <v>169</v>
-      </c>
-      <c r="U19" s="32" t="s">
-        <v>171</v>
       </c>
       <c r="V19" s="72"/>
       <c r="W19" s="70" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="Z19" s="3"/>
       <c r="AE19" s="43"/>
@@ -2672,7 +2717,7 @@
       </c>
       <c r="V20" s="73"/>
       <c r="W20" s="70" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Z20" s="3"/>
     </row>
@@ -2701,7 +2746,7 @@
       <c r="V21" s="73"/>
       <c r="W21" s="69"/>
       <c r="Z21" s="43" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="AA21" s="43"/>
       <c r="AB21" s="43"/>
@@ -2714,7 +2759,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2778,7 +2823,7 @@
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V23" s="73"/>
       <c r="W23" s="70"/>
@@ -2811,13 +2856,13 @@
         <v>56</v>
       </c>
       <c r="U24" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="V24" s="73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W24" s="70" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
@@ -2890,7 +2935,7 @@
       </c>
       <c r="V26" s="78"/>
       <c r="W26" s="69" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2924,7 +2969,7 @@
       <c r="U27" s="12"/>
       <c r="V27" s="75"/>
       <c r="W27" s="69" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3008,7 +3053,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>1</v>
@@ -3018,18 +3063,18 @@
       <c r="V30" s="72"/>
       <c r="W30" s="69"/>
       <c r="Z30" s="3" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="AC30" s="3"/>
       <c r="AD30" s="45" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="AE30" s="45"/>
       <c r="AF30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG30" s="45" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3063,10 +3108,10 @@
         <v>76</v>
       </c>
       <c r="V31" s="72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="W31" s="70" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="Y31" s="3"/>
       <c r="Z31" s="33"/>
@@ -3075,13 +3120,13 @@
       </c>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AG31" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:33" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
@@ -3112,24 +3157,24 @@
         <v>56</v>
       </c>
       <c r="U32" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V32" s="72"/>
       <c r="W32" s="70" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AG32" s="45" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3164,18 +3209,18 @@
       <c r="W33" s="69"/>
       <c r="X33" s="3"/>
       <c r="Z33" s="3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG33" s="45" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3242,13 +3287,13 @@
         <v>56</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="V35" s="76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W35" s="70" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3" t="s">
@@ -3257,10 +3302,10 @@
       <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF35" s="3" t="s">
         <v>1</v>
@@ -3325,7 +3370,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>1</v>
@@ -3370,16 +3415,16 @@
         <v>56</v>
       </c>
       <c r="U38" s="13" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="V38" s="73" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="W38" s="70" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="AA38" s="62" t="s">
-        <v>238</v>
+        <v>328</v>
       </c>
       <c r="AB38" s="62"/>
       <c r="AC38" s="62"/>
@@ -3387,13 +3432,13 @@
         <v>69</v>
       </c>
       <c r="AE38" s="62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF38" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG38" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3429,19 +3474,19 @@
       </c>
       <c r="V39" s="73"/>
       <c r="W39" s="70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="AD39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG39" s="105" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3476,19 +3521,19 @@
       <c r="W40" s="69"/>
       <c r="Y40" s="4"/>
       <c r="AA40" s="62" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="AB40" s="62"/>
       <c r="AC40" s="62"/>
       <c r="AD40" s="62" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="AE40" s="62"/>
       <c r="AF40" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG40" s="107" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3522,23 +3567,23 @@
         <v>75</v>
       </c>
       <c r="V41" s="73" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="W41" s="70" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="AA41" s="80"/>
       <c r="AB41" s="105" t="s">
         <v>23</v>
       </c>
       <c r="AE41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF41" t="s">
         <v>2</v>
       </c>
       <c r="AG41" s="106" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:34" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -3569,24 +3614,24 @@
         <v>56</v>
       </c>
       <c r="U42" s="13" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="V42" s="75"/>
       <c r="W42" s="70" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="AA42" s="62"/>
       <c r="AB42" t="s">
         <v>27</v>
       </c>
       <c r="AE42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF42" t="s">
         <v>2</v>
       </c>
       <c r="AG42" s="106" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3617,24 +3662,24 @@
         <v>56</v>
       </c>
       <c r="U43" s="13" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="V43" s="75"/>
       <c r="W43" s="70" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="AA43" s="62"/>
       <c r="AB43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AE43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF43" t="s">
         <v>2</v>
       </c>
       <c r="AG43" s="106" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3643,7 +3688,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -3665,24 +3710,24 @@
         <v>56</v>
       </c>
       <c r="U44" s="13" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="V44" s="75"/>
       <c r="W44" s="70" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="AA44" s="62"/>
       <c r="AB44" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="AE44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF44" t="s">
         <v>2</v>
       </c>
       <c r="AG44" s="106" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:34" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
@@ -3691,7 +3736,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -3713,23 +3758,23 @@
         <v>56</v>
       </c>
       <c r="U45" s="13" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="V45" s="75"/>
       <c r="W45" s="70" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="AB45" t="s">
         <v>28</v>
       </c>
       <c r="AE45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF45" t="s">
         <v>2</v>
       </c>
       <c r="AG45" s="106" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3737,7 +3782,7 @@
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="5" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -3759,23 +3804,23 @@
         <v>56</v>
       </c>
       <c r="U46" s="13" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="V46" s="75"/>
       <c r="W46" s="70" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="AB46" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="AE46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF46" t="s">
         <v>2</v>
       </c>
       <c r="AG46" s="107" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3813,7 +3858,7 @@
       <c r="AF47" s="3"/>
       <c r="AG47" s="54"/>
     </row>
-    <row r="48" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3841,13 +3886,13 @@
         <v>56</v>
       </c>
       <c r="U48" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="V48" s="73" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="W48" s="70" t="s">
-        <v>203</v>
+        <v>321</v>
       </c>
     </row>
     <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3879,19 +3924,19 @@
       <c r="V49" s="75"/>
       <c r="W49" s="70"/>
       <c r="AA49" s="62" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="AB49" s="62"/>
       <c r="AC49" s="62"/>
       <c r="AD49" s="62" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="AE49" s="62"/>
       <c r="AF49" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG49" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3915,7 +3960,7 @@
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S50" s="6" t="s">
         <v>1</v>
@@ -3927,7 +3972,7 @@
       <c r="V50" s="75"/>
       <c r="W50" s="69"/>
     </row>
-    <row r="51" spans="1:34" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3955,16 +4000,16 @@
         <v>56</v>
       </c>
       <c r="U51" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V51" s="73" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="W51" s="70" t="s">
-        <v>199</v>
+        <v>322</v>
       </c>
       <c r="AB51" s="109" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="AC51" s="62"/>
       <c r="AD51" s="109" t="s">
@@ -3975,7 +4020,7 @@
         <v>2</v>
       </c>
       <c r="AG51" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4006,11 +4051,11 @@
         <v>38</v>
       </c>
       <c r="U52" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V52" s="73"/>
       <c r="W52" s="69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AB52" s="62"/>
       <c r="AC52" s="62"/>
@@ -4047,24 +4092,24 @@
       </c>
       <c r="U53" s="13"/>
       <c r="V53" s="73" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="W53" s="70" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="AB53" s="109" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="AC53" s="62"/>
       <c r="AD53" s="62"/>
       <c r="AE53" s="109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF53" s="109" t="s">
         <v>2</v>
       </c>
       <c r="AG53" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4088,18 +4133,18 @@
       <c r="P54" s="4"/>
       <c r="Q54" s="4"/>
       <c r="R54" s="5" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="S54" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T54" s="4"/>
       <c r="U54" s="13" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="V54" s="73"/>
       <c r="W54" s="69" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="AB54"/>
       <c r="AE54"/>
@@ -4131,28 +4176,28 @@
         <v>1</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="U55" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="V55" s="73" t="s">
         <v>306</v>
       </c>
-      <c r="V55" s="73" t="s">
-        <v>322</v>
-      </c>
       <c r="W55" s="70" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="AB55" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="AE55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF55" t="s">
         <v>2</v>
       </c>
       <c r="AG55" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4176,18 +4221,18 @@
       <c r="P56" s="4"/>
       <c r="Q56" s="4"/>
       <c r="R56" s="5" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="S56" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T56" s="4"/>
       <c r="U56" s="13" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="V56" s="73"/>
       <c r="W56" s="70" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="AB56"/>
       <c r="AE56"/>
@@ -4219,31 +4264,31 @@
         <v>1</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="U57" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="V57" s="73" t="s">
         <v>307</v>
       </c>
-      <c r="V57" s="73" t="s">
-        <v>323</v>
-      </c>
       <c r="W57" s="70" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="AB57" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="AE57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF57" t="s">
         <v>2</v>
       </c>
       <c r="AG57" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:34" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -4273,22 +4318,22 @@
         <v>73</v>
       </c>
       <c r="V58" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W58" s="70" t="s">
-        <v>200</v>
+        <v>323</v>
       </c>
       <c r="AB58" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="AE58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF58" t="s">
         <v>2</v>
       </c>
       <c r="AG58" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4321,16 +4366,16 @@
       <c r="V59" s="75"/>
       <c r="W59" s="70"/>
       <c r="AB59" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="AE59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF59" t="s">
         <v>2</v>
       </c>
       <c r="AG59" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4386,7 +4431,7 @@
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S61" s="6" t="s">
         <v>1</v>
@@ -4396,7 +4441,7 @@
       <c r="V61" s="75"/>
       <c r="W61" s="69"/>
       <c r="AA61" s="62" t="s">
-        <v>268</v>
+        <v>326</v>
       </c>
       <c r="AB61" s="62"/>
       <c r="AC61" s="62"/>
@@ -4404,7 +4449,7 @@
         <v>69</v>
       </c>
       <c r="AE61" s="62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF61" s="62" t="s">
         <v>2</v>
@@ -4413,7 +4458,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="D62" s="4"/>
@@ -4441,10 +4486,10 @@
         <v>74</v>
       </c>
       <c r="V62" s="72" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="W62" s="70" t="s">
-        <v>201</v>
+        <v>324</v>
       </c>
       <c r="AA62" s="62"/>
       <c r="AB62" s="62"/>
@@ -4480,11 +4525,11 @@
         <v>38</v>
       </c>
       <c r="U63" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V63" s="72"/>
       <c r="W63" s="70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AA63" s="62"/>
       <c r="AB63" s="62"/>
@@ -4525,7 +4570,7 @@
       <c r="V64" s="73"/>
       <c r="W64" s="69"/>
       <c r="AA64" s="62" t="s">
-        <v>269</v>
+        <v>327</v>
       </c>
       <c r="AB64" s="62"/>
       <c r="AC64" s="62"/>
@@ -4533,7 +4578,7 @@
         <v>69</v>
       </c>
       <c r="AE64" s="62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF64" s="62" t="s">
         <v>2</v>
@@ -4631,7 +4676,7 @@
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S67" s="4" t="s">
         <v>1</v>
@@ -4648,7 +4693,7 @@
       <c r="AF67" s="3"/>
       <c r="AG67" s="54"/>
     </row>
-    <row r="68" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="D68" s="4"/>
@@ -4678,10 +4723,10 @@
         <v>71</v>
       </c>
       <c r="V68" s="76" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="W68" s="70" t="s">
-        <v>218</v>
+        <v>325</v>
       </c>
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
@@ -4718,11 +4763,11 @@
         <v>1.2.752.129.2.1.4.1</v>
       </c>
       <c r="U69" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V69" s="72"/>
       <c r="W69" s="70" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
@@ -4788,7 +4833,7 @@
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
       <c r="R71" s="5" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>1</v>
@@ -4830,27 +4875,27 @@
         <v>56</v>
       </c>
       <c r="U72" s="14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="V72" s="73" t="s">
         <v>83</v>
       </c>
       <c r="W72" s="70" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="X72" s="36"/>
       <c r="Z72" s="3" t="s">
         <v>84</v>
       </c>
       <c r="AD72" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AE72" s="3"/>
       <c r="AF72" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG72" s="45" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4917,7 +4962,7 @@
       <c r="U74" s="84"/>
       <c r="V74" s="75"/>
       <c r="W74" s="70" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="X74" s="17"/>
       <c r="AA74" s="3" t="s">
@@ -4926,16 +4971,16 @@
       <c r="AB74" s="3"/>
       <c r="AC74" s="3"/>
       <c r="AD74" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE74" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF74" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG74" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4992,17 +5037,17 @@
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
       <c r="R76" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T76" s="4"/>
       <c r="U76" s="13" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="V76" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W76" s="70"/>
       <c r="X76" s="17"/>
@@ -5040,11 +5085,11 @@
       </c>
       <c r="V77" s="73"/>
       <c r="W77" s="70" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="X77" s="17"/>
       <c r="AA77" s="3" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="AD77" s="3" t="s">
         <v>69</v>
@@ -5054,7 +5099,7 @@
         <v>2</v>
       </c>
       <c r="AG77" s="54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5090,22 +5135,22 @@
       </c>
       <c r="V78" s="78"/>
       <c r="W78" s="69" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="X78" s="56"/>
       <c r="AA78" s="3" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="AB78" s="3"/>
       <c r="AD78" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE78" s="3"/>
       <c r="AF78" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG78" s="54" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5161,17 +5206,17 @@
       <c r="P80" s="4"/>
       <c r="Q80" s="4"/>
       <c r="R80" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="S80" s="5" t="s">
         <v>1</v>
       </c>
       <c r="T80" s="4"/>
       <c r="U80" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="V80" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W80" s="69"/>
       <c r="X80" s="36"/>
@@ -5209,7 +5254,7 @@
       </c>
       <c r="V81" s="75"/>
       <c r="W81" s="70" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="X81" s="59"/>
       <c r="AE81" s="3"/>
@@ -5247,7 +5292,7 @@
       </c>
       <c r="V82" s="73"/>
       <c r="W82" s="69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="X82" s="57"/>
       <c r="AE82" s="3"/>
@@ -5279,11 +5324,11 @@
       </c>
       <c r="T83" s="4"/>
       <c r="U83" s="20" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="V83" s="73"/>
       <c r="W83" s="70" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="X83" s="57"/>
       <c r="AE83" s="3"/>
@@ -5310,7 +5355,7 @@
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
       <c r="R84" s="5" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="S84" s="5" t="s">
         <v>1</v>
@@ -5321,7 +5366,7 @@
       <c r="U84" s="20"/>
       <c r="V84" s="73"/>
       <c r="W84" s="69" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="X84" s="57"/>
       <c r="AE84" s="3"/>
@@ -5357,10 +5402,10 @@
         <v>98</v>
       </c>
       <c r="V85" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W85" s="70" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="X85" s="17"/>
       <c r="AB85" s="3"/>
@@ -5426,10 +5471,10 @@
       </c>
       <c r="T87" s="4"/>
       <c r="U87" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="V87" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W87" s="69"/>
       <c r="X87" s="3"/>
@@ -5460,25 +5505,25 @@
         <v>310866003</v>
       </c>
       <c r="U88" s="20" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="V88" s="76"/>
       <c r="W88" s="70" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="Z88" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC88" s="3"/>
       <c r="AD88" s="3"/>
       <c r="AE88" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF88" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG88" s="54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5511,7 +5556,7 @@
       </c>
       <c r="V89" s="73"/>
       <c r="W89" s="70" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5577,7 +5622,7 @@
       <c r="U91" s="13"/>
       <c r="V91" s="73"/>
       <c r="W91" s="70" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="Y91" s="3"/>
       <c r="Z91" s="62"/>
@@ -5591,7 +5636,7 @@
     </row>
     <row r="92" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B92" s="55" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C92" s="56"/>
       <c r="D92" s="55"/>
@@ -5614,7 +5659,7 @@
       </c>
       <c r="T92" s="55"/>
       <c r="U92" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="V92" s="73"/>
       <c r="W92" s="70"/>
@@ -5630,7 +5675,7 @@
     <row r="93" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B93" s="55"/>
       <c r="C93" s="56" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D93" s="55"/>
       <c r="E93" s="56"/>
@@ -5681,7 +5726,7 @@
       </c>
       <c r="T94" s="55"/>
       <c r="U94" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="V94" s="73"/>
       <c r="W94" s="70"/>
@@ -5714,30 +5759,30 @@
         <v>56</v>
       </c>
       <c r="U95" s="114" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="V95" s="76" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W95" s="115" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="X95" s="3"/>
       <c r="Z95" s="3" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="AA95" s="3"/>
       <c r="AB95" s="3"/>
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
       <c r="AE95" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF95" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG95" s="116" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5771,7 +5816,7 @@
       </c>
       <c r="V96" s="73"/>
       <c r="W96" s="70" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AG96" s="36"/>
     </row>
@@ -5843,10 +5888,10 @@
         <v>1</v>
       </c>
       <c r="T98" s="55" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="V98" s="73"/>
       <c r="W98" s="70"/>
@@ -5854,7 +5899,7 @@
     </row>
     <row r="99" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B99" s="55" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C99" s="56"/>
       <c r="D99" s="56"/>
@@ -5878,7 +5923,7 @@
       <c r="T99" s="55"/>
       <c r="U99" s="11"/>
       <c r="V99" s="73" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="W99" s="70"/>
       <c r="AG99" s="36"/>
@@ -5886,7 +5931,7 @@
     <row r="100" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B100" s="55"/>
       <c r="C100" s="56" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D100" s="56"/>
       <c r="E100" s="56"/>
@@ -5907,7 +5952,7 @@
         <v>1</v>
       </c>
       <c r="T100" s="55" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="U100" s="11"/>
       <c r="V100" s="73"/>
@@ -5974,7 +6019,7 @@
       </c>
       <c r="V102" s="73"/>
       <c r="W102" s="70" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="AG102" s="36"/>
     </row>
@@ -6005,11 +6050,11 @@
         <v>56</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="V103" s="73"/>
       <c r="W103" s="70" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="AG103" s="36"/>
     </row>
@@ -6091,10 +6136,10 @@
       <c r="V106" s="75"/>
       <c r="W106" s="86"/>
       <c r="Y106" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD106" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AG106" s="36"/>
     </row>
@@ -6213,7 +6258,7 @@
     </row>
     <row r="111" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B111" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -6419,7 +6464,7 @@
       </c>
       <c r="T117" s="4"/>
       <c r="U117" s="83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V117" s="79"/>
       <c r="W117" s="69"/>
@@ -6457,11 +6502,11 @@
         <v>439401001</v>
       </c>
       <c r="U118" s="83" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V118" s="79"/>
       <c r="W118" s="70" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="X118" s="3"/>
       <c r="Z118" s="3"/>
@@ -6483,12 +6528,12 @@
         <v>1</v>
       </c>
       <c r="T119" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U119" s="32"/>
       <c r="V119" s="76"/>
       <c r="W119" s="70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="X119" s="3"/>
       <c r="Z119" s="3"/>
@@ -6526,7 +6571,7 @@
       <c r="U120" s="83"/>
       <c r="V120" s="79"/>
       <c r="W120" s="70" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="X120" s="3"/>
       <c r="Z120" s="3"/>
@@ -6542,7 +6587,7 @@
       <c r="E121" s="5"/>
       <c r="F121" s="56"/>
       <c r="G121" s="56" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -6559,12 +6604,12 @@
         <v>1</v>
       </c>
       <c r="T121" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="U121" s="83"/>
       <c r="V121" s="79"/>
       <c r="W121" s="70" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X121" s="3"/>
       <c r="Z121" s="3"/>
@@ -6593,14 +6638,14 @@
       <c r="P122" s="5"/>
       <c r="Q122" s="5"/>
       <c r="R122" s="5" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="S122" s="5" t="s">
         <v>2</v>
       </c>
       <c r="T122" s="80"/>
       <c r="U122" s="85" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="V122" s="79"/>
       <c r="W122" s="86"/>
@@ -6703,7 +6748,7 @@
         <v>1</v>
       </c>
       <c r="T125" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U125" s="61"/>
       <c r="V125" s="79"/>
@@ -6764,7 +6809,7 @@
       <c r="P127" s="4"/>
       <c r="Q127" s="4"/>
       <c r="R127" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="S127" s="6" t="s">
         <v>1</v>
@@ -6803,16 +6848,16 @@
         <v>56</v>
       </c>
       <c r="U128" s="20" t="s">
-        <v>221</v>
+        <v>340</v>
       </c>
       <c r="V128" s="76"/>
       <c r="W128" s="70" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="X128" s="46"/>
       <c r="Y128" s="112"/>
     </row>
-    <row r="129" spans="1:33" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:33" s="46" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -6840,30 +6885,30 @@
         <v>56</v>
       </c>
       <c r="U129" s="20"/>
-      <c r="V129" s="79" t="s">
-        <v>100</v>
+      <c r="V129" s="76" t="s">
+        <v>337</v>
       </c>
       <c r="W129" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Y129" s="2"/>
       <c r="Z129" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
       <c r="AC129" s="2"/>
       <c r="AD129" s="62" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="AE129" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF129" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG129" s="54" t="s">
-        <v>173</v>
+        <v>333</v>
       </c>
     </row>
     <row r="130" spans="1:33" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -6894,14 +6939,30 @@
         <v>54</v>
       </c>
       <c r="U130" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V130" s="79"/>
       <c r="W130" s="70" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X130" s="3"/>
       <c r="Y130" s="2"/>
+      <c r="Z130" s="121" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3"/>
+      <c r="AC130" s="3"/>
+      <c r="AD130" s="3"/>
+      <c r="AE130" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF130" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG130" s="45" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="131" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
@@ -6913,7 +6974,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="4"/>
       <c r="I131" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
@@ -6928,14 +6989,14 @@
         <v>1</v>
       </c>
       <c r="T131" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="U131" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V131" s="79"/>
       <c r="W131" s="70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="132" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -6959,7 +7020,7 @@
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
       <c r="R132" s="5" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="S132" s="4" t="s">
         <v>2</v>
@@ -6970,26 +7031,26 @@
         <v>99</v>
       </c>
       <c r="W132" s="69" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="X132" s="3"/>
       <c r="Z132" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA132" s="3"/>
       <c r="AB132" s="3"/>
       <c r="AC132" s="3"/>
       <c r="AD132" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE132" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF132" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG132" s="54" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7001,7 +7062,7 @@
       <c r="F133" s="4"/>
       <c r="G133" s="5"/>
       <c r="H133" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
@@ -7013,7 +7074,7 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="S133" s="5" t="s">
         <v>2</v>
@@ -7024,20 +7085,20 @@
       <c r="W133" s="70"/>
       <c r="X133" s="3"/>
       <c r="Z133" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AA133" s="3"/>
       <c r="AB133" s="3"/>
       <c r="AC133" s="3"/>
       <c r="AD133" s="3" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="AE133" s="3"/>
       <c r="AF133" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG133" s="54" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="134" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7062,11 +7123,17 @@
       <c r="Q134" s="4"/>
       <c r="R134" s="4"/>
       <c r="S134" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T134" s="5"/>
-      <c r="U134" s="61"/>
-      <c r="V134" s="76"/>
+        <v>2</v>
+      </c>
+      <c r="T134" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U134" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="V134" s="76" t="s">
+        <v>164</v>
+      </c>
       <c r="W134" s="70"/>
       <c r="X134" s="3"/>
       <c r="Y134" s="3"/>
@@ -7078,13 +7145,13 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
       <c r="AE134" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF134" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG134" s="54" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
     </row>
     <row r="135" spans="1:33" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7096,10 +7163,10 @@
       <c r="F135" s="4"/>
       <c r="G135" s="5"/>
       <c r="H135" s="4"/>
-      <c r="J135" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K135" s="4"/>
+      <c r="I135" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J135" s="5"/>
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
@@ -7107,20 +7174,20 @@
       <c r="P135" s="4"/>
       <c r="Q135" s="4"/>
       <c r="R135" s="4"/>
-      <c r="S135" s="6" t="s">
-        <v>1</v>
+      <c r="S135" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="T135" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="U135" s="61" t="s">
-        <v>102</v>
+      <c r="U135" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="V135" s="76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W135" s="70" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="Z135" s="3"/>
       <c r="AA135" s="3" t="s">
@@ -7130,13 +7197,13 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
       <c r="AE135" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF135" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG135" s="54" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" spans="1:33" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
@@ -7148,10 +7215,10 @@
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
       <c r="H136" s="5"/>
-      <c r="J136" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K136" s="5"/>
+      <c r="I136" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J136" s="5"/>
       <c r="L136" s="5"/>
       <c r="M136" s="5"/>
       <c r="N136" s="5"/>
@@ -7159,20 +7226,18 @@
       <c r="P136" s="5"/>
       <c r="Q136" s="5"/>
       <c r="R136" s="5"/>
-      <c r="S136" s="6" t="s">
-        <v>1</v>
+      <c r="S136" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="T136" s="5" t="s">
         <v>56</v>
       </c>
       <c r="U136" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="V136" s="76" t="s">
-        <v>167</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="V136" s="76"/>
       <c r="W136" s="70" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="Y136" s="55"/>
       <c r="Z136" s="3"/>
@@ -7183,13 +7248,13 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
       <c r="AE136" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF136" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG136" s="3" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="137" spans="1:33" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7201,10 +7266,10 @@
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
-      <c r="J137" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K137" s="5"/>
+      <c r="I137" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="J137" s="5"/>
       <c r="L137" s="5"/>
       <c r="M137" s="5"/>
       <c r="N137" s="5"/>
@@ -7212,38 +7277,38 @@
       <c r="P137" s="5"/>
       <c r="Q137" s="5"/>
       <c r="R137" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S137" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T137" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="U137" s="20" t="s">
-        <v>178</v>
+      <c r="U137" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="V137" s="79"/>
       <c r="W137" s="70" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="X137" s="3"/>
       <c r="Y137" s="55"/>
       <c r="Z137" s="3"/>
       <c r="AA137" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AB137" s="3"/>
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
       <c r="AE137" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF137" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG137" s="54" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
     </row>
     <row r="138" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7255,11 +7320,9 @@
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
       <c r="H138" s="5"/>
-      <c r="I138" s="2"/>
-      <c r="J138" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="K138" s="5"/>
+      <c r="I138" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="L138" s="5"/>
       <c r="M138" s="5"/>
       <c r="N138" s="5"/>
@@ -7268,30 +7331,30 @@
       <c r="Q138" s="5"/>
       <c r="R138" s="5"/>
       <c r="S138" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T138" s="5" t="s">
         <v>56</v>
       </c>
       <c r="U138" s="13" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="V138" s="76"/>
       <c r="W138" s="70" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="Y138" s="55"/>
       <c r="AA138" s="3" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="AE138" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF138" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG138" s="3" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="139" spans="1:33" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
@@ -7303,7 +7366,9 @@
       <c r="F139" s="4"/>
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
-      <c r="I139" s="4"/>
+      <c r="I139" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
@@ -7313,26 +7378,30 @@
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
       <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
+      <c r="S139" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T139" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="U139" s="13"/>
       <c r="V139" s="76"/>
       <c r="W139" s="70"/>
       <c r="Y139" s="55"/>
       <c r="AA139" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="AE139" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF139" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG139" s="45" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="140" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="140" spans="1:33" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
@@ -7340,8 +7409,10 @@
       <c r="E140" s="5"/>
       <c r="F140" s="4"/>
       <c r="G140" s="5"/>
-      <c r="H140" s="5"/>
-      <c r="I140" s="5"/>
+      <c r="H140" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
@@ -7351,11 +7422,15 @@
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
-      <c r="S140" s="6"/>
+      <c r="S140" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="T140" s="5"/>
       <c r="U140" s="13"/>
       <c r="V140" s="76"/>
-      <c r="W140" s="70"/>
+      <c r="W140" s="70" t="s">
+        <v>341</v>
+      </c>
       <c r="Y140" s="55"/>
       <c r="AC140" s="2"/>
       <c r="AD140" s="2"/>
@@ -7363,7 +7438,7 @@
       <c r="AF140" s="2"/>
       <c r="AG140" s="36"/>
     </row>
-    <row r="141" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A141" s="5"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -7371,22 +7446,32 @@
       <c r="E141" s="5"/>
       <c r="F141" s="4"/>
       <c r="G141" s="5"/>
-      <c r="H141" s="80"/>
-      <c r="I141" s="5"/>
-      <c r="J141" s="5"/>
-      <c r="K141" s="5"/>
-      <c r="L141" s="5"/>
-      <c r="M141" s="5"/>
-      <c r="N141" s="5"/>
-      <c r="O141" s="5"/>
-      <c r="P141" s="5"/>
-      <c r="Q141" s="5"/>
-      <c r="R141" s="5"/>
-      <c r="S141" s="5"/>
-      <c r="T141" s="5"/>
-      <c r="U141" s="13"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="80" t="s">
+        <v>171</v>
+      </c>
+      <c r="J141" s="80"/>
+      <c r="K141" s="80"/>
+      <c r="L141" s="80"/>
+      <c r="M141" s="80"/>
+      <c r="N141" s="80"/>
+      <c r="O141" s="80"/>
+      <c r="P141" s="80"/>
+      <c r="Q141" s="80"/>
+      <c r="R141" s="80"/>
+      <c r="S141" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="T141" s="80" t="s">
+        <v>334</v>
+      </c>
+      <c r="U141" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="V141" s="76"/>
-      <c r="W141" s="70"/>
+      <c r="W141" s="70" t="s">
+        <v>342</v>
+      </c>
       <c r="Y141" s="55"/>
       <c r="AC141" s="2"/>
       <c r="AD141" s="2"/>
@@ -7402,8 +7487,10 @@
       <c r="E142" s="5"/>
       <c r="F142" s="4"/>
       <c r="G142" s="5"/>
-      <c r="H142" s="4"/>
-      <c r="I142" s="4"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="J142" s="5"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
@@ -7413,6 +7500,9 @@
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
+      <c r="S142" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="T142" s="2"/>
       <c r="U142" s="13"/>
       <c r="V142" s="76"/>
@@ -7436,7 +7526,9 @@
       <c r="G143" s="5"/>
       <c r="H143" s="4"/>
       <c r="I143" s="2"/>
-      <c r="J143" s="5"/>
+      <c r="J143" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="K143" s="5"/>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
@@ -7445,6 +7537,9 @@
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
+      <c r="S143" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="T143" s="5"/>
       <c r="U143" s="61"/>
       <c r="V143" s="76"/>
@@ -7458,7 +7553,7 @@
       <c r="AF143" s="62"/>
       <c r="AG143" s="87"/>
     </row>
-    <row r="144" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A144" s="5"/>
       <c r="B144" s="5"/>
       <c r="C144" s="4"/>
@@ -7469,7 +7564,9 @@
       <c r="H144" s="4"/>
       <c r="I144" s="2"/>
       <c r="J144" s="5"/>
-      <c r="K144" s="4"/>
+      <c r="K144" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="L144" s="4"/>
       <c r="M144" s="4"/>
       <c r="N144" s="4"/>
@@ -7477,10 +7574,19 @@
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
-      <c r="T144" s="4"/>
-      <c r="U144" s="13"/>
+      <c r="S144" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T144" s="122">
+        <v>90734009</v>
+      </c>
+      <c r="U144" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="V144" s="76"/>
-      <c r="W144" s="70"/>
+      <c r="W144" s="70" t="s">
+        <v>343</v>
+      </c>
       <c r="Z144" s="62"/>
       <c r="AA144" s="62"/>
       <c r="AB144" s="62"/>
@@ -7490,7 +7596,7 @@
       <c r="AF144" s="62"/>
       <c r="AG144" s="87"/>
     </row>
-    <row r="145" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -7501,7 +7607,9 @@
       <c r="H145" s="4"/>
       <c r="I145" s="2"/>
       <c r="J145" s="5"/>
-      <c r="K145" s="4"/>
+      <c r="K145" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="L145" s="4"/>
       <c r="M145" s="4"/>
       <c r="N145" s="4"/>
@@ -7509,13 +7617,22 @@
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
-      <c r="T145" s="4"/>
-      <c r="U145" s="13"/>
+      <c r="S145" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T145" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="U145" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="V145" s="76"/>
-      <c r="W145" s="70"/>
+      <c r="W145" s="70" t="s">
+        <v>344</v>
+      </c>
       <c r="Y145" s="2"/>
     </row>
-    <row r="146" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -7526,6 +7643,9 @@
       <c r="H146" s="4"/>
       <c r="I146" s="2"/>
       <c r="J146" s="2"/>
+      <c r="K146" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="L146" s="2"/>
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
@@ -7533,15 +7653,25 @@
       <c r="P146" s="2"/>
       <c r="Q146" s="2"/>
       <c r="R146" s="2"/>
-      <c r="U146" s="14"/>
+      <c r="S146" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T146" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="U146" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="V146" s="76"/>
-      <c r="W146" s="70"/>
+      <c r="W146" s="70" t="s">
+        <v>345</v>
+      </c>
       <c r="Y146" s="2"/>
       <c r="Z146" s="2"/>
       <c r="AA146" s="2"/>
       <c r="AG146" s="65"/>
     </row>
-    <row r="147" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="5"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -7552,6 +7682,9 @@
       <c r="H147" s="4"/>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
+      <c r="K147" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="L147" s="2"/>
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
@@ -7559,10 +7692,19 @@
       <c r="P147" s="2"/>
       <c r="Q147" s="2"/>
       <c r="R147" s="2"/>
-      <c r="T147" s="2"/>
-      <c r="U147" s="14"/>
+      <c r="S147" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T147" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="U147" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="V147" s="76"/>
-      <c r="W147" s="70"/>
+      <c r="W147" s="70" t="s">
+        <v>346</v>
+      </c>
       <c r="Y147" s="2"/>
       <c r="Z147" s="2"/>
       <c r="AA147" s="2"/>
@@ -7572,52 +7714,42 @@
       <c r="A148" s="5"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="D148" s="2"/>
       <c r="E148" s="4"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-      <c r="H148" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
-      <c r="M148" s="4"/>
-      <c r="N148" s="4"/>
-      <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
-      <c r="Q148" s="4"/>
-      <c r="R148" s="4"/>
+      <c r="F148" s="5"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K148" s="5"/>
+      <c r="L148" s="2"/>
+      <c r="M148" s="2"/>
+      <c r="N148" s="2"/>
+      <c r="O148" s="2"/>
+      <c r="P148" s="2"/>
+      <c r="Q148" s="2"/>
+      <c r="R148" s="3" t="s">
+        <v>339</v>
+      </c>
       <c r="S148" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="T148" s="5"/>
-      <c r="U148" s="60" t="s">
-        <v>103</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T148" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="U148" s="13"/>
       <c r="V148" s="76" t="s">
-        <v>126</v>
+        <v>336</v>
       </c>
       <c r="W148" s="70" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z148" s="3" t="s">
-        <v>117</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="Y148" s="2"/>
+      <c r="Z148" s="2"/>
       <c r="AA148" s="2"/>
-      <c r="AB148" s="2"/>
-      <c r="AC148" s="2"/>
-      <c r="AD148" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE148" s="2"/>
-      <c r="AF148" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG148" s="55" t="s">
-        <v>123</v>
-      </c>
+      <c r="AG148" s="65"/>
     </row>
     <row r="149" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" s="5"/>
@@ -7627,10 +7759,10 @@
       <c r="E149" s="4"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-      <c r="H149" s="5"/>
-      <c r="I149" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="H149" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="I149" s="4"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
@@ -7641,30 +7773,46 @@
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
       <c r="S149" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T149" s="5" t="s">
-        <v>213</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="T149" s="5"/>
       <c r="U149" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="V149" s="76"/>
+        <v>102</v>
+      </c>
+      <c r="V149" s="76" t="s">
+        <v>332</v>
+      </c>
       <c r="W149" s="70" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="150" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="4"/>
+        <v>215</v>
+      </c>
+      <c r="Z149" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA149" s="2"/>
+      <c r="AB149" s="2"/>
+      <c r="AC149" s="2"/>
+      <c r="AD149" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE149" s="2"/>
+      <c r="AF149" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG149" s="55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="150" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A150" s="5"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
-      <c r="F150" s="5"/>
-      <c r="G150" s="5"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
       <c r="H150" s="5"/>
       <c r="I150" s="5" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
@@ -7678,31 +7826,46 @@
       <c r="S150" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T150" s="4"/>
-      <c r="U150" s="13"/>
+      <c r="T150" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="U150" s="60" t="s">
+        <v>169</v>
+      </c>
       <c r="V150" s="76"/>
-      <c r="W150" s="70"/>
-      <c r="Z150" s="2"/>
-    </row>
-    <row r="151" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W150" s="70" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="151" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
-      <c r="J151" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S151" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T151" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="U151" s="20"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="5"/>
+      <c r="H151" s="5"/>
+      <c r="I151" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J151" s="4"/>
+      <c r="K151" s="4"/>
+      <c r="L151" s="4"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="4"/>
+      <c r="S151" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T151" s="4"/>
+      <c r="U151" s="13"/>
       <c r="V151" s="76"/>
       <c r="W151" s="70"/>
-      <c r="Y151" s="3"/>
+      <c r="Z151" s="2"/>
     </row>
     <row r="152" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
@@ -7711,17 +7874,17 @@
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
       <c r="J152" s="3" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="S152" s="5" t="s">
         <v>1</v>
       </c>
       <c r="T152" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="U152" s="13"/>
-      <c r="V152" s="79"/>
-      <c r="W152" s="69"/>
+        <v>100</v>
+      </c>
+      <c r="U152" s="20"/>
+      <c r="V152" s="76"/>
+      <c r="W152" s="70"/>
       <c r="Y152" s="3"/>
     </row>
     <row r="153" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7730,106 +7893,82 @@
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
-      <c r="J153" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K153" s="4"/>
-      <c r="S153" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U153" s="61"/>
-      <c r="V153" s="78"/>
+      <c r="J153" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S153" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T153" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="U153" s="13"/>
+      <c r="V153" s="79"/>
       <c r="W153" s="69"/>
       <c r="Y153" s="3"/>
     </row>
-    <row r="154" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
-      <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="J154" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K154" s="4"/>
       <c r="S154" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="T154" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="U154" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="V154" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="W154" s="70" t="s">
-        <v>314</v>
-      </c>
+      <c r="U154" s="61"/>
+      <c r="V154" s="78"/>
+      <c r="W154" s="69"/>
       <c r="Y154" s="3"/>
-      <c r="AA154" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="AB154" s="3"/>
-      <c r="AC154" s="3"/>
-      <c r="AD154" s="3"/>
-      <c r="AE154" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF154" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG154" s="54" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="155" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="5"/>
-      <c r="H155" s="6"/>
-      <c r="I155" s="5"/>
+      <c r="I155" s="3"/>
       <c r="J155" s="4"/>
       <c r="K155" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L155" s="4"/>
-      <c r="M155" s="4"/>
-      <c r="N155" s="4"/>
-      <c r="O155" s="4"/>
-      <c r="P155" s="4"/>
-      <c r="Q155" s="4"/>
-      <c r="R155" s="4"/>
+        <v>26</v>
+      </c>
       <c r="S155" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T155" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="U155" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="V155" s="78"/>
+        <v>56</v>
+      </c>
+      <c r="U155" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="V155" s="72" t="s">
+        <v>158</v>
+      </c>
       <c r="W155" s="70" t="s">
-        <v>179</v>
+        <v>298</v>
       </c>
       <c r="Y155" s="3"/>
-      <c r="Z155" s="33"/>
-      <c r="AA155" s="3"/>
+      <c r="AA155" s="121" t="s">
+        <v>267</v>
+      </c>
       <c r="AB155" s="3"/>
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
-      <c r="AE155" s="3"/>
-      <c r="AF155" s="3"/>
-      <c r="AG155" s="65"/>
-    </row>
-    <row r="156" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE155" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF155" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG155" s="54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="156" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
@@ -7839,10 +7978,10 @@
       <c r="G156" s="5"/>
       <c r="H156" s="6"/>
       <c r="I156" s="5"/>
-      <c r="J156" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K156" s="4"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="L156" s="4"/>
       <c r="M156" s="4"/>
       <c r="N156" s="4"/>
@@ -7850,18 +7989,30 @@
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
       <c r="R156" s="4"/>
-      <c r="S156" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T156" s="3"/>
-      <c r="U156" s="20"/>
+      <c r="S156" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T156" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="U156" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="V156" s="78"/>
-      <c r="W156" s="69"/>
+      <c r="W156" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y156" s="3"/>
+      <c r="Z156" s="33"/>
       <c r="AA156" s="3"/>
+      <c r="AB156" s="3"/>
+      <c r="AC156" s="3"/>
+      <c r="AD156" s="3"/>
       <c r="AE156" s="3"/>
-      <c r="AG156" s="36"/>
-    </row>
-    <row r="157" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AF156" s="3"/>
+      <c r="AG156" s="65"/>
+    </row>
+    <row r="157" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
@@ -7871,10 +8022,11 @@
       <c r="G157" s="5"/>
       <c r="H157" s="6"/>
       <c r="I157" s="5"/>
-      <c r="K157" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="L157" s="5"/>
+      <c r="J157" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K157" s="4"/>
+      <c r="L157" s="4"/>
       <c r="M157" s="4"/>
       <c r="N157" s="4"/>
       <c r="O157" s="4"/>
@@ -7884,18 +8036,15 @@
       <c r="S157" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T157" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="U157" s="20" t="s">
-        <v>171</v>
-      </c>
+      <c r="T157" s="3"/>
+      <c r="U157" s="20"/>
       <c r="V157" s="78"/>
-      <c r="W157" s="70" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="158" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W157" s="69"/>
+      <c r="AA157" s="3"/>
+      <c r="AE157" s="3"/>
+      <c r="AG157" s="36"/>
+    </row>
+    <row r="158" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -7905,8 +8054,9 @@
       <c r="G158" s="5"/>
       <c r="H158" s="6"/>
       <c r="I158" s="5"/>
-      <c r="J158" s="4"/>
-      <c r="K158" s="5"/>
+      <c r="K158" s="5" t="s">
+        <v>309</v>
+      </c>
       <c r="L158" s="5"/>
       <c r="M158" s="4"/>
       <c r="N158" s="4"/>
@@ -7914,16 +8064,19 @@
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
       <c r="R158" s="4"/>
-      <c r="S158" s="4"/>
-      <c r="T158" s="4"/>
-      <c r="U158" s="61"/>
+      <c r="S158" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T158" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="U158" s="20" t="s">
+        <v>169</v>
+      </c>
       <c r="V158" s="78"/>
-      <c r="W158" s="70"/>
-      <c r="AA158" s="3"/>
-      <c r="AD158" s="62"/>
-      <c r="AE158" s="3"/>
-      <c r="AF158" s="3"/>
-      <c r="AG158" s="54"/>
+      <c r="W158" s="70" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="159" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
@@ -7935,8 +8088,8 @@
       <c r="G159" s="5"/>
       <c r="H159" s="6"/>
       <c r="I159" s="5"/>
-      <c r="J159" s="5"/>
-      <c r="K159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="5"/>
       <c r="L159" s="5"/>
       <c r="M159" s="4"/>
       <c r="N159" s="4"/>
@@ -7946,9 +8099,14 @@
       <c r="R159" s="4"/>
       <c r="S159" s="4"/>
       <c r="T159" s="4"/>
-      <c r="U159" s="20"/>
-      <c r="V159" s="79"/>
+      <c r="U159" s="61"/>
+      <c r="V159" s="78"/>
       <c r="W159" s="70"/>
+      <c r="AA159" s="3"/>
+      <c r="AD159" s="62"/>
+      <c r="AE159" s="3"/>
+      <c r="AF159" s="3"/>
+      <c r="AG159" s="54"/>
     </row>
     <row r="160" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4"/>
@@ -7960,9 +8118,9 @@
       <c r="G160" s="5"/>
       <c r="H160" s="6"/>
       <c r="I160" s="5"/>
-      <c r="J160" s="4"/>
+      <c r="J160" s="5"/>
       <c r="K160" s="3"/>
-      <c r="L160" s="4"/>
+      <c r="L160" s="5"/>
       <c r="M160" s="4"/>
       <c r="N160" s="4"/>
       <c r="O160" s="4"/>
@@ -7972,15 +8130,8 @@
       <c r="S160" s="4"/>
       <c r="T160" s="4"/>
       <c r="U160" s="20"/>
-      <c r="V160" s="73"/>
+      <c r="V160" s="79"/>
       <c r="W160" s="70"/>
-      <c r="AA160" s="62"/>
-      <c r="AB160" s="62"/>
-      <c r="AC160" s="62"/>
-      <c r="AD160" s="62"/>
-      <c r="AE160" s="62"/>
-      <c r="AF160" s="62"/>
-      <c r="AG160" s="87"/>
     </row>
     <row r="161" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4"/>
@@ -7988,12 +8139,12 @@
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="5"/>
-      <c r="K161" s="4"/>
+      <c r="F161" s="5"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="5"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="3"/>
       <c r="L161" s="4"/>
       <c r="M161" s="4"/>
       <c r="N161" s="4"/>
@@ -8001,12 +8152,11 @@
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
       <c r="R161" s="4"/>
-      <c r="S161" s="5"/>
+      <c r="S161" s="4"/>
       <c r="T161" s="4"/>
       <c r="U161" s="20"/>
       <c r="V161" s="73"/>
-      <c r="W161" s="69"/>
-      <c r="Z161" s="3"/>
+      <c r="W161" s="70"/>
       <c r="AA161" s="62"/>
       <c r="AB161" s="62"/>
       <c r="AC161" s="62"/>
@@ -8025,8 +8175,8 @@
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="5"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="4"/>
       <c r="L162" s="4"/>
       <c r="M162" s="4"/>
       <c r="N162" s="4"/>
@@ -8034,12 +8184,12 @@
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
       <c r="R162" s="4"/>
-      <c r="S162" s="6"/>
+      <c r="S162" s="5"/>
       <c r="T162" s="4"/>
-      <c r="U162" s="61"/>
-      <c r="V162" s="79"/>
+      <c r="U162" s="20"/>
+      <c r="V162" s="73"/>
       <c r="W162" s="69"/>
-      <c r="X162" s="55"/>
+      <c r="Z162" s="3"/>
       <c r="AA162" s="62"/>
       <c r="AB162" s="62"/>
       <c r="AC162" s="62"/>
@@ -8058,7 +8208,7 @@
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
-      <c r="J163" s="5"/>
+      <c r="J163" s="4"/>
       <c r="K163" s="5"/>
       <c r="L163" s="4"/>
       <c r="M163" s="4"/>
@@ -8067,9 +8217,9 @@
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
       <c r="R163" s="4"/>
-      <c r="S163" s="5"/>
+      <c r="S163" s="6"/>
       <c r="T163" s="4"/>
-      <c r="U163" s="13"/>
+      <c r="U163" s="61"/>
       <c r="V163" s="79"/>
       <c r="W163" s="69"/>
       <c r="X163" s="55"/>
@@ -8091,8 +8241,8 @@
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="5"/>
       <c r="L164" s="4"/>
       <c r="M164" s="4"/>
       <c r="N164" s="4"/>
@@ -8100,11 +8250,12 @@
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
       <c r="R164" s="4"/>
-      <c r="S164" s="4"/>
+      <c r="S164" s="5"/>
       <c r="T164" s="4"/>
-      <c r="U164" s="21"/>
-      <c r="V164" s="73"/>
+      <c r="U164" s="13"/>
+      <c r="V164" s="79"/>
       <c r="W164" s="69"/>
+      <c r="X164" s="55"/>
       <c r="AA164" s="62"/>
       <c r="AB164" s="62"/>
       <c r="AC164" s="62"/>
@@ -8115,12 +8266,13 @@
     </row>
     <row r="165" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
       <c r="F165" s="4"/>
       <c r="G165" s="4"/>
-      <c r="H165" s="6"/>
+      <c r="H165" s="4"/>
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
@@ -8131,10 +8283,10 @@
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
       <c r="R165" s="4"/>
-      <c r="S165" s="6"/>
+      <c r="S165" s="4"/>
       <c r="T165" s="4"/>
       <c r="U165" s="21"/>
-      <c r="V165" s="78"/>
+      <c r="V165" s="73"/>
       <c r="W165" s="69"/>
       <c r="AA165" s="62"/>
       <c r="AB165" s="62"/>
@@ -8142,30 +8294,30 @@
       <c r="AD165" s="62"/>
       <c r="AE165" s="62"/>
       <c r="AF165" s="62"/>
-      <c r="AG165" s="95"/>
+      <c r="AG165" s="87"/>
     </row>
     <row r="166" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4"/>
-      <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
       <c r="F166" s="4"/>
-      <c r="G166" s="5"/>
-      <c r="H166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="6"/>
       <c r="I166" s="4"/>
-      <c r="J166" s="5"/>
+      <c r="J166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
       <c r="M166" s="4"/>
       <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
       <c r="R166" s="4"/>
-      <c r="S166" s="4"/>
+      <c r="S166" s="6"/>
       <c r="T166" s="4"/>
-      <c r="U166" s="14"/>
-      <c r="V166" s="73"/>
+      <c r="U166" s="21"/>
+      <c r="V166" s="78"/>
       <c r="W166" s="69"/>
       <c r="AA166" s="62"/>
       <c r="AB166" s="62"/>
@@ -8173,7 +8325,7 @@
       <c r="AD166" s="62"/>
       <c r="AE166" s="62"/>
       <c r="AF166" s="62"/>
-      <c r="AG166" s="96"/>
+      <c r="AG166" s="95"/>
     </row>
     <row r="167" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4"/>
@@ -8182,20 +8334,21 @@
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
       <c r="F167" s="4"/>
-      <c r="G167" s="4"/>
-      <c r="H167" s="5"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="4"/>
       <c r="I167" s="4"/>
-      <c r="J167" s="4"/>
+      <c r="J167" s="5"/>
       <c r="K167" s="4"/>
-      <c r="L167" s="5"/>
+      <c r="L167" s="4"/>
       <c r="M167" s="4"/>
       <c r="N167" s="4"/>
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
       <c r="R167" s="4"/>
-      <c r="S167" s="3"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
       <c r="U167" s="14"/>
-      <c r="V167" s="76"/>
+      <c r="V167" s="73"/>
       <c r="W167" s="69"/>
       <c r="AA167" s="62"/>
       <c r="AB167" s="62"/>
@@ -8214,18 +8367,18 @@
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
       <c r="H168" s="5"/>
-      <c r="I168" s="5"/>
+      <c r="I168" s="4"/>
       <c r="J168" s="4"/>
+      <c r="K168" s="4"/>
       <c r="L168" s="5"/>
-      <c r="M168" s="5"/>
+      <c r="M168" s="4"/>
       <c r="N168" s="4"/>
       <c r="P168" s="4"/>
       <c r="Q168" s="4"/>
       <c r="R168" s="4"/>
       <c r="S168" s="3"/>
-      <c r="T168" s="5"/>
-      <c r="U168" s="61"/>
-      <c r="V168" s="73"/>
+      <c r="U168" s="14"/>
+      <c r="V168" s="76"/>
       <c r="W168" s="69"/>
       <c r="AA168" s="62"/>
       <c r="AB168" s="62"/>
@@ -8233,34 +8386,42 @@
       <c r="AD168" s="62"/>
       <c r="AE168" s="62"/>
       <c r="AF168" s="62"/>
-      <c r="AG168" s="87"/>
+      <c r="AG168" s="96"/>
     </row>
     <row r="169" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
+      <c r="D169" s="4"/>
       <c r="E169" s="4"/>
       <c r="F169" s="4"/>
       <c r="G169" s="4"/>
-      <c r="H169" s="4"/>
-      <c r="I169" s="4"/>
+      <c r="H169" s="5"/>
+      <c r="I169" s="5"/>
       <c r="J169" s="4"/>
       <c r="L169" s="5"/>
-      <c r="M169" s="4"/>
+      <c r="M169" s="5"/>
       <c r="N169" s="4"/>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
       <c r="R169" s="4"/>
       <c r="S169" s="3"/>
-      <c r="T169" s="4"/>
-      <c r="U169" s="13"/>
+      <c r="T169" s="5"/>
+      <c r="U169" s="61"/>
       <c r="V169" s="73"/>
       <c r="W169" s="69"/>
-      <c r="AG169" s="36"/>
+      <c r="AA169" s="62"/>
+      <c r="AB169" s="62"/>
+      <c r="AC169" s="62"/>
+      <c r="AD169" s="62"/>
+      <c r="AE169" s="62"/>
+      <c r="AF169" s="62"/>
+      <c r="AG169" s="87"/>
     </row>
     <row r="170" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
       <c r="E170" s="4"/>
       <c r="F170" s="4"/>
       <c r="G170" s="4"/>
@@ -8276,7 +8437,7 @@
       <c r="S170" s="3"/>
       <c r="T170" s="4"/>
       <c r="U170" s="13"/>
-      <c r="V170" s="76"/>
+      <c r="V170" s="73"/>
       <c r="W170" s="69"/>
       <c r="AG170" s="36"/>
     </row>
@@ -8289,22 +8450,26 @@
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
       <c r="J171" s="4"/>
-      <c r="M171" s="3"/>
+      <c r="L171" s="5"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
       <c r="P171" s="4"/>
       <c r="Q171" s="4"/>
       <c r="R171" s="4"/>
       <c r="S171" s="3"/>
-      <c r="T171" s="3"/>
-      <c r="U171" s="14"/>
-      <c r="V171" s="79"/>
+      <c r="T171" s="4"/>
+      <c r="U171" s="13"/>
+      <c r="V171" s="76"/>
       <c r="W171" s="69"/>
       <c r="AG171" s="36"/>
     </row>
     <row r="172" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4"/>
-      <c r="D172" s="4"/>
+      <c r="B172" s="4"/>
       <c r="E172" s="4"/>
-      <c r="H172" s="5"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="M172" s="3"/>
@@ -8312,35 +8477,31 @@
       <c r="Q172" s="4"/>
       <c r="R172" s="4"/>
       <c r="S172" s="3"/>
+      <c r="T172" s="3"/>
       <c r="U172" s="14"/>
-      <c r="V172" s="73"/>
+      <c r="V172" s="79"/>
       <c r="W172" s="69"/>
       <c r="AG172" s="36"/>
     </row>
     <row r="173" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="4"/>
-      <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
-      <c r="H173" s="4"/>
-      <c r="I173" s="5"/>
+      <c r="H173" s="5"/>
+      <c r="I173" s="4"/>
       <c r="J173" s="4"/>
-      <c r="K173" s="4"/>
-      <c r="L173" s="4"/>
-      <c r="M173" s="4"/>
+      <c r="M173" s="3"/>
       <c r="P173" s="4"/>
       <c r="Q173" s="4"/>
       <c r="R173" s="4"/>
-      <c r="S173" s="4"/>
-      <c r="T173" s="5"/>
-      <c r="U173" s="20"/>
-      <c r="V173" s="75"/>
+      <c r="S173" s="3"/>
+      <c r="U173" s="14"/>
+      <c r="V173" s="73"/>
       <c r="W173" s="69"/>
       <c r="AG173" s="36"/>
     </row>
     <row r="174" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4"/>
-      <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -8354,13 +8515,15 @@
       <c r="Q174" s="4"/>
       <c r="R174" s="4"/>
       <c r="S174" s="4"/>
-      <c r="U174" s="60"/>
+      <c r="T174" s="5"/>
+      <c r="U174" s="20"/>
       <c r="V174" s="75"/>
       <c r="W174" s="69"/>
       <c r="AG174" s="36"/>
     </row>
     <row r="175" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -8374,14 +8537,13 @@
       <c r="Q175" s="4"/>
       <c r="R175" s="4"/>
       <c r="S175" s="4"/>
-      <c r="U175" s="14"/>
-      <c r="V175" s="74"/>
+      <c r="U175" s="60"/>
+      <c r="V175" s="75"/>
       <c r="W175" s="69"/>
       <c r="AG175" s="36"/>
     </row>
     <row r="176" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -8395,9 +8557,8 @@
       <c r="Q176" s="4"/>
       <c r="R176" s="4"/>
       <c r="S176" s="4"/>
-      <c r="T176" s="3"/>
-      <c r="U176" s="21"/>
-      <c r="V176" s="79"/>
+      <c r="U176" s="14"/>
+      <c r="V176" s="74"/>
       <c r="W176" s="69"/>
       <c r="AG176" s="36"/>
     </row>
@@ -8407,10 +8568,8 @@
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
-      <c r="F177" s="4"/>
-      <c r="G177" s="4"/>
-      <c r="H177" s="5"/>
-      <c r="I177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="5"/>
       <c r="J177" s="4"/>
       <c r="K177" s="4"/>
       <c r="L177" s="4"/>
@@ -8419,9 +8578,9 @@
       <c r="Q177" s="4"/>
       <c r="R177" s="4"/>
       <c r="S177" s="4"/>
-      <c r="T177" s="4"/>
-      <c r="U177" s="13"/>
-      <c r="V177" s="74"/>
+      <c r="T177" s="3"/>
+      <c r="U177" s="21"/>
+      <c r="V177" s="79"/>
       <c r="W177" s="69"/>
       <c r="AG177" s="36"/>
     </row>
@@ -8433,21 +8592,19 @@
       <c r="E178" s="4"/>
       <c r="F178" s="4"/>
       <c r="G178" s="4"/>
-      <c r="H178" s="4"/>
+      <c r="H178" s="5"/>
       <c r="I178" s="4"/>
       <c r="J178" s="4"/>
       <c r="K178" s="4"/>
       <c r="L178" s="4"/>
       <c r="M178" s="4"/>
-      <c r="N178" s="4"/>
-      <c r="O178" s="4"/>
       <c r="P178" s="4"/>
       <c r="Q178" s="4"/>
       <c r="R178" s="4"/>
       <c r="S178" s="4"/>
       <c r="T178" s="4"/>
       <c r="U178" s="13"/>
-      <c r="V178" s="93"/>
+      <c r="V178" s="74"/>
       <c r="W178" s="69"/>
       <c r="AG178" s="36"/>
     </row>
@@ -8472,8 +8629,8 @@
       <c r="R179" s="4"/>
       <c r="S179" s="4"/>
       <c r="T179" s="4"/>
-      <c r="U179" s="14"/>
-      <c r="V179" s="75"/>
+      <c r="U179" s="13"/>
+      <c r="V179" s="93"/>
       <c r="W179" s="69"/>
       <c r="AG179" s="36"/>
     </row>
@@ -8498,8 +8655,8 @@
       <c r="R180" s="4"/>
       <c r="S180" s="4"/>
       <c r="T180" s="4"/>
-      <c r="U180" s="21"/>
-      <c r="V180" s="78"/>
+      <c r="U180" s="14"/>
+      <c r="V180" s="75"/>
       <c r="W180" s="69"/>
       <c r="AG180" s="36"/>
     </row>
@@ -8525,7 +8682,7 @@
       <c r="S181" s="4"/>
       <c r="T181" s="4"/>
       <c r="U181" s="21"/>
-      <c r="V181" s="75"/>
+      <c r="V181" s="78"/>
       <c r="W181" s="69"/>
       <c r="AG181" s="36"/>
     </row>
@@ -8536,7 +8693,7 @@
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
       <c r="F182" s="4"/>
-      <c r="G182" s="5"/>
+      <c r="G182" s="4"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
       <c r="J182" s="4"/>
@@ -8547,9 +8704,11 @@
       <c r="O182" s="4"/>
       <c r="P182" s="4"/>
       <c r="Q182" s="4"/>
+      <c r="R182" s="4"/>
+      <c r="S182" s="4"/>
       <c r="T182" s="4"/>
       <c r="U182" s="21"/>
-      <c r="V182" s="78"/>
+      <c r="V182" s="75"/>
       <c r="W182" s="69"/>
       <c r="AG182" s="36"/>
     </row>
@@ -8560,8 +8719,8 @@
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
       <c r="F183" s="4"/>
-      <c r="G183" s="4"/>
-      <c r="H183" s="5"/>
+      <c r="G183" s="5"/>
+      <c r="H183" s="4"/>
       <c r="I183" s="4"/>
       <c r="J183" s="4"/>
       <c r="K183" s="4"/>
@@ -8573,7 +8732,7 @@
       <c r="Q183" s="4"/>
       <c r="T183" s="4"/>
       <c r="U183" s="21"/>
-      <c r="V183" s="74"/>
+      <c r="V183" s="78"/>
       <c r="W183" s="69"/>
       <c r="AG183" s="36"/>
     </row>
@@ -8596,7 +8755,7 @@
       <c r="P184" s="4"/>
       <c r="Q184" s="4"/>
       <c r="T184" s="4"/>
-      <c r="U184" s="61"/>
+      <c r="U184" s="21"/>
       <c r="V184" s="74"/>
       <c r="W184" s="69"/>
       <c r="AG184" s="36"/>
@@ -8620,8 +8779,8 @@
       <c r="P185" s="4"/>
       <c r="Q185" s="4"/>
       <c r="T185" s="4"/>
-      <c r="U185" s="12"/>
-      <c r="V185" s="75"/>
+      <c r="U185" s="61"/>
+      <c r="V185" s="74"/>
       <c r="W185" s="69"/>
       <c r="AG185" s="36"/>
     </row>
@@ -8633,8 +8792,8 @@
       <c r="E186" s="4"/>
       <c r="F186" s="4"/>
       <c r="G186" s="4"/>
-      <c r="H186" s="4"/>
-      <c r="I186" s="5"/>
+      <c r="H186" s="5"/>
+      <c r="I186" s="4"/>
       <c r="J186" s="4"/>
       <c r="K186" s="4"/>
       <c r="L186" s="4"/>
@@ -8645,8 +8804,8 @@
       <c r="Q186" s="4"/>
       <c r="T186" s="4"/>
       <c r="U186" s="12"/>
-      <c r="V186" s="57"/>
-      <c r="W186" s="56"/>
+      <c r="V186" s="75"/>
+      <c r="W186" s="69"/>
       <c r="AG186" s="36"/>
     </row>
     <row r="187" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8681,8 +8840,8 @@
       <c r="E188" s="4"/>
       <c r="F188" s="4"/>
       <c r="G188" s="4"/>
-      <c r="H188" s="5"/>
-      <c r="I188" s="4"/>
+      <c r="H188" s="4"/>
+      <c r="I188" s="5"/>
       <c r="J188" s="4"/>
       <c r="K188" s="4"/>
       <c r="L188" s="4"/>
@@ -8693,8 +8852,9 @@
       <c r="Q188" s="4"/>
       <c r="T188" s="4"/>
       <c r="U188" s="12"/>
-      <c r="V188" s="58"/>
-      <c r="W188" s="58"/>
+      <c r="V188" s="57"/>
+      <c r="W188" s="56"/>
+      <c r="AG188" s="36"/>
     </row>
     <row r="189" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="4"/>
@@ -8704,8 +8864,8 @@
       <c r="E189" s="4"/>
       <c r="F189" s="4"/>
       <c r="G189" s="4"/>
-      <c r="H189" s="4"/>
-      <c r="I189" s="5"/>
+      <c r="H189" s="5"/>
+      <c r="I189" s="4"/>
       <c r="J189" s="4"/>
       <c r="K189" s="4"/>
       <c r="L189" s="4"/>
@@ -8715,9 +8875,9 @@
       <c r="P189" s="4"/>
       <c r="Q189" s="4"/>
       <c r="T189" s="4"/>
-      <c r="U189" s="11"/>
-      <c r="V189" s="59"/>
-      <c r="W189" s="17"/>
+      <c r="U189" s="12"/>
+      <c r="V189" s="58"/>
+      <c r="W189" s="58"/>
     </row>
     <row r="190" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="4"/>
@@ -8737,7 +8897,8 @@
       <c r="O190" s="4"/>
       <c r="P190" s="4"/>
       <c r="Q190" s="4"/>
-      <c r="U190" s="14"/>
+      <c r="T190" s="4"/>
+      <c r="U190" s="11"/>
       <c r="V190" s="59"/>
       <c r="W190" s="17"/>
     </row>
@@ -8747,6 +8908,8 @@
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
       <c r="H191" s="4"/>
       <c r="I191" s="5"/>
       <c r="J191" s="4"/>
@@ -8757,7 +8920,6 @@
       <c r="O191" s="4"/>
       <c r="P191" s="4"/>
       <c r="Q191" s="4"/>
-      <c r="T191" s="5"/>
       <c r="U191" s="14"/>
       <c r="V191" s="59"/>
       <c r="W191" s="17"/>
@@ -8768,8 +8930,6 @@
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
-      <c r="F192" s="4"/>
-      <c r="G192" s="4"/>
       <c r="H192" s="4"/>
       <c r="I192" s="5"/>
       <c r="J192" s="4"/>
@@ -8780,8 +8940,8 @@
       <c r="O192" s="4"/>
       <c r="P192" s="4"/>
       <c r="Q192" s="4"/>
-      <c r="T192" s="4"/>
-      <c r="U192" s="12"/>
+      <c r="T192" s="5"/>
+      <c r="U192" s="14"/>
       <c r="V192" s="59"/>
       <c r="W192" s="17"/>
     </row>
@@ -8793,8 +8953,8 @@
       <c r="E193" s="4"/>
       <c r="F193" s="4"/>
       <c r="G193" s="4"/>
-      <c r="H193" s="5"/>
-      <c r="I193" s="4"/>
+      <c r="H193" s="4"/>
+      <c r="I193" s="5"/>
       <c r="J193" s="4"/>
       <c r="K193" s="4"/>
       <c r="L193" s="4"/>
@@ -8803,33 +8963,49 @@
       <c r="O193" s="4"/>
       <c r="P193" s="4"/>
       <c r="Q193" s="4"/>
-      <c r="S193" s="4"/>
       <c r="T193" s="4"/>
-      <c r="U193" s="11"/>
-      <c r="V193" s="65"/>
-      <c r="W193" s="36"/>
+      <c r="U193" s="12"/>
+      <c r="V193" s="59"/>
+      <c r="W193" s="17"/>
     </row>
     <row r="194" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="4"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
-      <c r="I194" s="3"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="4"/>
+      <c r="H194" s="5"/>
+      <c r="I194" s="4"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="4"/>
+      <c r="L194" s="4"/>
+      <c r="M194" s="4"/>
+      <c r="N194" s="4"/>
+      <c r="O194" s="4"/>
+      <c r="P194" s="4"/>
+      <c r="Q194" s="4"/>
+      <c r="S194" s="4"/>
+      <c r="T194" s="4"/>
       <c r="U194" s="11"/>
-      <c r="V194" s="59"/>
-      <c r="W194" s="17"/>
+      <c r="V194" s="65"/>
+      <c r="W194" s="36"/>
     </row>
     <row r="195" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="4"/>
       <c r="B195" s="4"/>
-      <c r="J195" s="3"/>
-      <c r="U195" s="14"/>
+      <c r="C195" s="4"/>
+      <c r="I195" s="3"/>
+      <c r="U195" s="11"/>
       <c r="V195" s="59"/>
       <c r="W195" s="17"/>
     </row>
     <row r="196" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="4"/>
       <c r="B196" s="4"/>
-      <c r="U196" s="9"/>
+      <c r="J196" s="3"/>
+      <c r="U196" s="14"/>
       <c r="V196" s="59"/>
       <c r="W196" s="17"/>
     </row>
@@ -8842,17 +9018,18 @@
     </row>
     <row r="198" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="4"/>
+      <c r="B198" s="4"/>
       <c r="U198" s="9"/>
-      <c r="V198" s="57"/>
-      <c r="W198" s="56"/>
-    </row>
-    <row r="199" spans="1:33" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V198" s="59"/>
+      <c r="W198" s="17"/>
+    </row>
+    <row r="199" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="4"/>
       <c r="U199" s="9"/>
-      <c r="V199" s="58"/>
-      <c r="W199" s="58"/>
-    </row>
-    <row r="200" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V199" s="57"/>
+      <c r="W199" s="56"/>
+    </row>
+    <row r="200" spans="1:33" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="4"/>
       <c r="U200" s="9"/>
       <c r="V200" s="58"/>
@@ -8861,43 +9038,35 @@
     <row r="201" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="4"/>
       <c r="U201" s="9"/>
-      <c r="V201" s="59"/>
-      <c r="W201" s="17"/>
+      <c r="V201" s="58"/>
+      <c r="W201" s="58"/>
     </row>
     <row r="202" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="4"/>
       <c r="U202" s="9"/>
-      <c r="V202" s="57"/>
-      <c r="W202" s="56"/>
+      <c r="V202" s="59"/>
+      <c r="W202" s="17"/>
     </row>
     <row r="203" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="4"/>
       <c r="U203" s="9"/>
       <c r="V203" s="57"/>
       <c r="W203" s="56"/>
     </row>
     <row r="204" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="U204" s="9"/>
-      <c r="V204" s="58"/>
-      <c r="W204" s="58"/>
+      <c r="V204" s="57"/>
+      <c r="W204" s="56"/>
     </row>
     <row r="205" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="U205" s="9"/>
-      <c r="V205" s="65"/>
-      <c r="W205" s="36"/>
+      <c r="V205" s="58"/>
+      <c r="W205" s="58"/>
     </row>
     <row r="206" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="U206" s="9"/>
       <c r="V206" s="65"/>
       <c r="W206" s="36"/>
-      <c r="Y206" s="1"/>
-      <c r="Z206" s="1"/>
-      <c r="AA206" s="1"/>
-      <c r="AB206" s="1"/>
-      <c r="AC206" s="1"/>
-      <c r="AD206" s="1"/>
-      <c r="AE206" s="1"/>
-      <c r="AF206" s="1"/>
-      <c r="AG206" s="1"/>
     </row>
     <row r="207" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="U207" s="9"/>
@@ -8956,23 +9125,6 @@
       <c r="AG210" s="1"/>
     </row>
     <row r="211" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
-      <c r="G211" s="1"/>
-      <c r="H211" s="1"/>
-      <c r="I211" s="1"/>
-      <c r="J211" s="1"/>
-      <c r="K211" s="1"/>
-      <c r="L211" s="1"/>
-      <c r="M211" s="1"/>
-      <c r="N211" s="1"/>
-      <c r="O211" s="1"/>
-      <c r="P211" s="1"/>
-      <c r="Q211" s="1"/>
-      <c r="R211" s="1"/>
-      <c r="S211" s="1"/>
-      <c r="T211" s="1"/>
       <c r="U211" s="9"/>
       <c r="V211" s="65"/>
       <c r="W211" s="36"/>
@@ -8987,7 +9139,6 @@
       <c r="AG211" s="1"/>
     </row>
     <row r="212" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C212" s="1"/>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
@@ -9037,7 +9188,7 @@
       <c r="R213" s="1"/>
       <c r="S213" s="1"/>
       <c r="T213" s="1"/>
-      <c r="U213" s="10"/>
+      <c r="U213" s="9"/>
       <c r="V213" s="65"/>
       <c r="W213" s="36"/>
       <c r="Y213" s="1"/>
@@ -9083,7 +9234,6 @@
       <c r="AG214" s="1"/>
     </row>
     <row r="215" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -9248,7 +9398,6 @@
       <c r="AG219" s="1"/>
     </row>
     <row r="220" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
@@ -9271,7 +9420,6 @@
       <c r="U220" s="10"/>
       <c r="V220" s="65"/>
       <c r="W220" s="36"/>
-      <c r="X220" s="1"/>
       <c r="Y220" s="1"/>
       <c r="Z220" s="1"/>
       <c r="AA220" s="1"/>
@@ -9282,9 +9430,44 @@
       <c r="AF220" s="1"/>
       <c r="AG220" s="1"/>
     </row>
-    <row r="221" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
+      <c r="H221" s="1"/>
+      <c r="I221" s="1"/>
+      <c r="J221" s="1"/>
+      <c r="K221" s="1"/>
+      <c r="L221" s="1"/>
+      <c r="M221" s="1"/>
+      <c r="N221" s="1"/>
+      <c r="O221" s="1"/>
+      <c r="P221" s="1"/>
+      <c r="Q221" s="1"/>
+      <c r="R221" s="1"/>
+      <c r="S221" s="1"/>
+      <c r="T221" s="1"/>
+      <c r="U221" s="10"/>
       <c r="V221" s="65"/>
       <c r="W221" s="36"/>
+      <c r="X221" s="1"/>
+      <c r="Y221" s="1"/>
+      <c r="Z221" s="1"/>
+      <c r="AA221" s="1"/>
+      <c r="AB221" s="1"/>
+      <c r="AC221" s="1"/>
+      <c r="AD221" s="1"/>
+      <c r="AE221" s="1"/>
+      <c r="AF221" s="1"/>
+      <c r="AG221" s="1"/>
+    </row>
+    <row r="222" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="V222" s="65"/>
+      <c r="W222" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Uppdaterat elementnamnet diagnosisType (till typeOfDiagnosis).
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/docs/Bilaga MIM_Mappningar_GetDiagnosis.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/healthcond/description/trunk/docs/Bilaga MIM_Mappningar_GetDiagnosis.xlsx
@@ -332,9 +332,6 @@
     <t>DiagnosisType</t>
   </si>
   <si>
-    <t>diagnosisType</t>
-  </si>
-  <si>
     <t>diagnosisTime</t>
   </si>
   <si>
@@ -911,9 +908,6 @@
 Annars: clinicalDocument.author.assignedAuthor.code.codeSystem = 1.2.752.129.2.2.1.4</t>
   </si>
   <si>
-    <t>diagnosisTypeEnum</t>
-  </si>
-  <si>
     <t>Tidpunkt då bedömningen gjordes.</t>
   </si>
   <si>
@@ -1067,6 +1061,12 @@
   </si>
   <si>
     <t>…section.entry.observation.entryRelationship.observation.value = diagnosisBody.chronicDiagnosis</t>
+  </si>
+  <si>
+    <t>typeOfDiagnosis</t>
+  </si>
+  <si>
+    <t>TypeOfDiagnosisEnum</t>
   </si>
 </sst>
 </file>
@@ -1582,6 +1582,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1590,12 +1596,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1947,8 +1947,8 @@
   <dimension ref="A1:AO222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA33" sqref="AA33"/>
+      <pane ySplit="6" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z130" sqref="Z130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2057,48 +2057,48 @@
       <c r="AO2" s="2"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="119"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="121"/>
       <c r="V3" s="89"/>
       <c r="W3" s="71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X3" s="63"/>
       <c r="Y3" s="63"/>
-      <c r="Z3" s="120" t="s">
+      <c r="Z3" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="120"/>
-      <c r="AB3" s="120"/>
-      <c r="AC3" s="120"/>
-      <c r="AD3" s="120"/>
-      <c r="AE3" s="120"/>
-      <c r="AF3" s="120"/>
-      <c r="AG3" s="120"/>
-      <c r="AH3" s="120"/>
-      <c r="AI3" s="120"/>
-      <c r="AJ3" s="120"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="122"/>
+      <c r="AC3" s="122"/>
+      <c r="AD3" s="122"/>
+      <c r="AE3" s="122"/>
+      <c r="AF3" s="122"/>
+      <c r="AG3" s="122"/>
+      <c r="AH3" s="122"/>
+      <c r="AI3" s="122"/>
+      <c r="AJ3" s="122"/>
     </row>
     <row r="4" spans="1:41" s="2" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
@@ -2159,20 +2159,20 @@
       <c r="P5" s="15"/>
       <c r="Q5" s="110"/>
       <c r="R5" s="111" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="29" t="s">
         <v>32</v>
       </c>
       <c r="V5" s="91" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="W5" s="67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X5" s="38"/>
       <c r="Y5" s="38"/>
@@ -2181,13 +2181,13 @@
       <c r="AB5" s="38"/>
       <c r="AC5" s="51"/>
       <c r="AD5" s="64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AE5" s="64" t="s">
         <v>67</v>
       </c>
       <c r="AF5" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AG5" s="64" t="s">
         <v>32</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="8" spans="1:41" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -2314,7 +2314,7 @@
       <c r="V9" s="75"/>
       <c r="W9" s="69"/>
       <c r="X9" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD9" s="46" t="s">
         <v>104</v>
@@ -2348,10 +2348,10 @@
       <c r="W10" s="69"/>
       <c r="X10" s="47"/>
       <c r="Y10" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD10" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2375,7 +2375,7 @@
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11" s="105" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S11" t="s">
         <v>1</v>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="V12" s="78"/>
       <c r="W12" s="70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:41" ht="25.5" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
       <c r="U13" s="7"/>
       <c r="V13" s="75"/>
       <c r="W13" s="70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2476,14 +2476,14 @@
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14" s="105" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S14" t="s">
         <v>1</v>
       </c>
       <c r="T14" s="17"/>
       <c r="U14" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V14" s="72"/>
       <c r="W14" s="70"/>
@@ -2517,27 +2517,27 @@
         <v>56</v>
       </c>
       <c r="U15" s="117" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="V15" s="73" t="s">
         <v>81</v>
       </c>
       <c r="W15" s="70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG15" s="45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:41" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="V16" s="104"/>
       <c r="W16" s="70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z16" s="3"/>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="V18" s="72"/>
       <c r="W18" s="70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z18" s="3"/>
       <c r="AE18" s="43"/>
@@ -2671,14 +2671,14 @@
         <v>1</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U19" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V19" s="72"/>
       <c r="W19" s="70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z19" s="3"/>
       <c r="AE19" s="43"/>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="V20" s="73"/>
       <c r="W20" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z20" s="3"/>
     </row>
@@ -2746,7 +2746,7 @@
       <c r="V21" s="73"/>
       <c r="W21" s="69"/>
       <c r="Z21" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA21" s="43"/>
       <c r="AB21" s="43"/>
@@ -2759,7 +2759,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V23" s="73"/>
       <c r="W23" s="70"/>
@@ -2856,13 +2856,13 @@
         <v>56</v>
       </c>
       <c r="U24" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="V24" s="73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W24" s="70" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="V26" s="78"/>
       <c r="W26" s="69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2969,7 +2969,7 @@
       <c r="U27" s="12"/>
       <c r="V27" s="75"/>
       <c r="W27" s="69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3053,7 +3053,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>1</v>
@@ -3063,18 +3063,18 @@
       <c r="V30" s="72"/>
       <c r="W30" s="69"/>
       <c r="Z30" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AC30" s="3"/>
       <c r="AD30" s="45" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AE30" s="45"/>
       <c r="AF30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG30" s="45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3108,10 +3108,10 @@
         <v>76</v>
       </c>
       <c r="V31" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W31" s="70" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Y31" s="3"/>
       <c r="Z31" s="33"/>
@@ -3120,13 +3120,13 @@
       </c>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AG31" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:33" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
@@ -3157,24 +3157,24 @@
         <v>56</v>
       </c>
       <c r="U32" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V32" s="72"/>
       <c r="W32" s="70" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AG32" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3209,18 +3209,18 @@
       <c r="W33" s="69"/>
       <c r="X33" s="3"/>
       <c r="Z33" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG33" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3287,13 +3287,13 @@
         <v>56</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="V35" s="76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W35" s="70" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3" t="s">
@@ -3302,10 +3302,10 @@
       <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF35" s="3" t="s">
         <v>1</v>
@@ -3370,7 +3370,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>1</v>
@@ -3415,16 +3415,16 @@
         <v>56</v>
       </c>
       <c r="U38" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="V38" s="73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W38" s="70" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA38" s="62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AB38" s="62"/>
       <c r="AC38" s="62"/>
@@ -3432,13 +3432,13 @@
         <v>69</v>
       </c>
       <c r="AE38" s="62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF38" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG38" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3474,19 +3474,19 @@
       </c>
       <c r="V39" s="73"/>
       <c r="W39" s="70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AD39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG39" s="105" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3521,19 +3521,19 @@
       <c r="W40" s="69"/>
       <c r="Y40" s="4"/>
       <c r="AA40" s="62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AB40" s="62"/>
       <c r="AC40" s="62"/>
       <c r="AD40" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AE40" s="62"/>
       <c r="AF40" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG40" s="107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3567,23 +3567,23 @@
         <v>75</v>
       </c>
       <c r="V41" s="73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W41" s="70" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA41" s="80"/>
       <c r="AB41" s="105" t="s">
         <v>23</v>
       </c>
       <c r="AE41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF41" t="s">
         <v>2</v>
       </c>
       <c r="AG41" s="106" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:34" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -3614,24 +3614,24 @@
         <v>56</v>
       </c>
       <c r="U42" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="V42" s="75"/>
       <c r="W42" s="70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AA42" s="62"/>
       <c r="AB42" t="s">
         <v>27</v>
       </c>
       <c r="AE42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF42" t="s">
         <v>2</v>
       </c>
       <c r="AG42" s="106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3662,24 +3662,24 @@
         <v>56</v>
       </c>
       <c r="U43" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="V43" s="75"/>
       <c r="W43" s="70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA43" s="62"/>
       <c r="AB43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF43" t="s">
         <v>2</v>
       </c>
       <c r="AG43" s="106" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3688,7 +3688,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -3710,24 +3710,24 @@
         <v>56</v>
       </c>
       <c r="U44" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="V44" s="75"/>
       <c r="W44" s="70" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AA44" s="62"/>
       <c r="AB44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AE44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF44" t="s">
         <v>2</v>
       </c>
       <c r="AG44" s="106" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:34" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
@@ -3736,7 +3736,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -3758,23 +3758,23 @@
         <v>56</v>
       </c>
       <c r="U45" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="V45" s="75"/>
       <c r="W45" s="70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AB45" t="s">
         <v>28</v>
       </c>
       <c r="AE45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF45" t="s">
         <v>2</v>
       </c>
       <c r="AG45" s="106" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3782,7 +3782,7 @@
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -3804,23 +3804,23 @@
         <v>56</v>
       </c>
       <c r="U46" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V46" s="75"/>
       <c r="W46" s="70" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AB46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AE46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF46" t="s">
         <v>2</v>
       </c>
       <c r="AG46" s="107" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3886,13 +3886,13 @@
         <v>56</v>
       </c>
       <c r="U48" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V48" s="73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="W48" s="70" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3924,19 +3924,19 @@
       <c r="V49" s="75"/>
       <c r="W49" s="70"/>
       <c r="AA49" s="62" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AB49" s="62"/>
       <c r="AC49" s="62"/>
       <c r="AD49" s="62" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AE49" s="62"/>
       <c r="AF49" s="62" t="s">
         <v>2</v>
       </c>
       <c r="AG49" s="45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3960,7 +3960,7 @@
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S50" s="6" t="s">
         <v>1</v>
@@ -4000,16 +4000,16 @@
         <v>56</v>
       </c>
       <c r="U51" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V51" s="73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W51" s="70" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AB51" s="109" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AC51" s="62"/>
       <c r="AD51" s="109" t="s">
@@ -4020,7 +4020,7 @@
         <v>2</v>
       </c>
       <c r="AG51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4051,11 +4051,11 @@
         <v>38</v>
       </c>
       <c r="U52" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V52" s="73"/>
       <c r="W52" s="69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB52" s="62"/>
       <c r="AC52" s="62"/>
@@ -4092,24 +4092,24 @@
       </c>
       <c r="U53" s="13"/>
       <c r="V53" s="73" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="W53" s="70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AB53" s="109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AC53" s="62"/>
       <c r="AD53" s="62"/>
       <c r="AE53" s="109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF53" s="109" t="s">
         <v>2</v>
       </c>
       <c r="AG53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4133,18 +4133,18 @@
       <c r="P54" s="4"/>
       <c r="Q54" s="4"/>
       <c r="R54" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="S54" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T54" s="4"/>
       <c r="U54" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V54" s="73"/>
       <c r="W54" s="69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB54"/>
       <c r="AE54"/>
@@ -4176,28 +4176,28 @@
         <v>1</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U55" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V55" s="73" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="W55" s="70" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AB55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AE55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF55" t="s">
         <v>2</v>
       </c>
       <c r="AG55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4221,18 +4221,18 @@
       <c r="P56" s="4"/>
       <c r="Q56" s="4"/>
       <c r="R56" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="S56" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T56" s="4"/>
       <c r="U56" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V56" s="73"/>
       <c r="W56" s="70" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB56"/>
       <c r="AE56"/>
@@ -4264,28 +4264,28 @@
         <v>1</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U57" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="V57" s="73" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="W57" s="70" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AB57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AE57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF57" t="s">
         <v>2</v>
       </c>
       <c r="AG57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:34" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -4318,22 +4318,22 @@
         <v>73</v>
       </c>
       <c r="V58" s="73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="W58" s="70" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AB58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AE58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF58" t="s">
         <v>2</v>
       </c>
       <c r="AG58" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4366,16 +4366,16 @@
       <c r="V59" s="75"/>
       <c r="W59" s="70"/>
       <c r="AB59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AE59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF59" t="s">
         <v>2</v>
       </c>
       <c r="AG59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4431,7 +4431,7 @@
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S61" s="6" t="s">
         <v>1</v>
@@ -4441,7 +4441,7 @@
       <c r="V61" s="75"/>
       <c r="W61" s="69"/>
       <c r="AA61" s="62" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AB61" s="62"/>
       <c r="AC61" s="62"/>
@@ -4449,7 +4449,7 @@
         <v>69</v>
       </c>
       <c r="AE61" s="62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF61" s="62" t="s">
         <v>2</v>
@@ -4486,10 +4486,10 @@
         <v>74</v>
       </c>
       <c r="V62" s="72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="W62" s="70" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AA62" s="62"/>
       <c r="AB62" s="62"/>
@@ -4525,11 +4525,11 @@
         <v>38</v>
       </c>
       <c r="U63" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V63" s="72"/>
       <c r="W63" s="70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AA63" s="62"/>
       <c r="AB63" s="62"/>
@@ -4570,7 +4570,7 @@
       <c r="V64" s="73"/>
       <c r="W64" s="69"/>
       <c r="AA64" s="62" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AB64" s="62"/>
       <c r="AC64" s="62"/>
@@ -4578,7 +4578,7 @@
         <v>69</v>
       </c>
       <c r="AE64" s="62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF64" s="62" t="s">
         <v>2</v>
@@ -4676,7 +4676,7 @@
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S67" s="4" t="s">
         <v>1</v>
@@ -4723,10 +4723,10 @@
         <v>71</v>
       </c>
       <c r="V68" s="76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="W68" s="70" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
@@ -4763,11 +4763,11 @@
         <v>1.2.752.129.2.1.4.1</v>
       </c>
       <c r="U69" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V69" s="72"/>
       <c r="W69" s="70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
@@ -4833,7 +4833,7 @@
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
       <c r="R71" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>1</v>
@@ -4875,27 +4875,27 @@
         <v>56</v>
       </c>
       <c r="U72" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V72" s="73" t="s">
         <v>83</v>
       </c>
       <c r="W72" s="70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X72" s="36"/>
       <c r="Z72" s="3" t="s">
         <v>84</v>
       </c>
       <c r="AD72" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE72" s="3"/>
       <c r="AF72" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG72" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4962,7 +4962,7 @@
       <c r="U74" s="84"/>
       <c r="V74" s="75"/>
       <c r="W74" s="70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="X74" s="17"/>
       <c r="AA74" s="3" t="s">
@@ -4971,16 +4971,16 @@
       <c r="AB74" s="3"/>
       <c r="AC74" s="3"/>
       <c r="AD74" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE74" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF74" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG74" s="54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5037,17 +5037,17 @@
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
       <c r="R76" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T76" s="4"/>
       <c r="U76" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="V76" s="73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W76" s="70"/>
       <c r="X76" s="17"/>
@@ -5085,11 +5085,11 @@
       </c>
       <c r="V77" s="73"/>
       <c r="W77" s="70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="X77" s="17"/>
       <c r="AA77" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD77" s="3" t="s">
         <v>69</v>
@@ -5099,7 +5099,7 @@
         <v>2</v>
       </c>
       <c r="AG77" s="54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5135,22 +5135,22 @@
       </c>
       <c r="V78" s="78"/>
       <c r="W78" s="69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X78" s="56"/>
       <c r="AA78" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AB78" s="3"/>
       <c r="AD78" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AE78" s="3"/>
       <c r="AF78" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG78" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5206,17 +5206,17 @@
       <c r="P80" s="4"/>
       <c r="Q80" s="4"/>
       <c r="R80" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S80" s="5" t="s">
         <v>1</v>
       </c>
       <c r="T80" s="4"/>
       <c r="U80" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V80" s="73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W80" s="69"/>
       <c r="X80" s="36"/>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="V81" s="75"/>
       <c r="W81" s="70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="X81" s="59"/>
       <c r="AE81" s="3"/>
@@ -5292,7 +5292,7 @@
       </c>
       <c r="V82" s="73"/>
       <c r="W82" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X82" s="57"/>
       <c r="AE82" s="3"/>
@@ -5324,11 +5324,11 @@
       </c>
       <c r="T83" s="4"/>
       <c r="U83" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V83" s="73"/>
       <c r="W83" s="70" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="X83" s="57"/>
       <c r="AE83" s="3"/>
@@ -5355,7 +5355,7 @@
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
       <c r="R84" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S84" s="5" t="s">
         <v>1</v>
@@ -5366,7 +5366,7 @@
       <c r="U84" s="20"/>
       <c r="V84" s="73"/>
       <c r="W84" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X84" s="57"/>
       <c r="AE84" s="3"/>
@@ -5402,10 +5402,10 @@
         <v>98</v>
       </c>
       <c r="V85" s="73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W85" s="70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X85" s="17"/>
       <c r="AB85" s="3"/>
@@ -5471,10 +5471,10 @@
       </c>
       <c r="T87" s="4"/>
       <c r="U87" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V87" s="73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W87" s="69"/>
       <c r="X87" s="3"/>
@@ -5505,25 +5505,25 @@
         <v>310866003</v>
       </c>
       <c r="U88" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="V88" s="76"/>
       <c r="W88" s="70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z88" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC88" s="3"/>
       <c r="AD88" s="3"/>
       <c r="AE88" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AF88" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG88" s="54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5556,7 +5556,7 @@
       </c>
       <c r="V89" s="73"/>
       <c r="W89" s="70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5622,7 +5622,7 @@
       <c r="U91" s="13"/>
       <c r="V91" s="73"/>
       <c r="W91" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y91" s="3"/>
       <c r="Z91" s="62"/>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="92" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B92" s="55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C92" s="56"/>
       <c r="D92" s="55"/>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="T92" s="55"/>
       <c r="U92" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V92" s="73"/>
       <c r="W92" s="70"/>
@@ -5675,7 +5675,7 @@
     <row r="93" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B93" s="55"/>
       <c r="C93" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D93" s="55"/>
       <c r="E93" s="56"/>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="T94" s="55"/>
       <c r="U94" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V94" s="73"/>
       <c r="W94" s="70"/>
@@ -5759,30 +5759,30 @@
         <v>56</v>
       </c>
       <c r="U95" s="114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V95" s="76" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W95" s="115" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="X95" s="3"/>
       <c r="Z95" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AA95" s="3"/>
       <c r="AB95" s="3"/>
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
       <c r="AE95" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF95" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG95" s="116" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="V96" s="73"/>
       <c r="W96" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AG96" s="36"/>
     </row>
@@ -5888,10 +5888,10 @@
         <v>1</v>
       </c>
       <c r="T98" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="U98" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="U98" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="V98" s="73"/>
       <c r="W98" s="70"/>
@@ -5899,7 +5899,7 @@
     </row>
     <row r="99" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B99" s="55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C99" s="56"/>
       <c r="D99" s="56"/>
@@ -5923,7 +5923,7 @@
       <c r="T99" s="55"/>
       <c r="U99" s="11"/>
       <c r="V99" s="73" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="W99" s="70"/>
       <c r="AG99" s="36"/>
@@ -5931,7 +5931,7 @@
     <row r="100" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B100" s="55"/>
       <c r="C100" s="56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D100" s="56"/>
       <c r="E100" s="56"/>
@@ -5952,7 +5952,7 @@
         <v>1</v>
       </c>
       <c r="T100" s="55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U100" s="11"/>
       <c r="V100" s="73"/>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="V102" s="73"/>
       <c r="W102" s="70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AG102" s="36"/>
     </row>
@@ -6050,11 +6050,11 @@
         <v>56</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V103" s="73"/>
       <c r="W103" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AG103" s="36"/>
     </row>
@@ -6136,7 +6136,7 @@
       <c r="V106" s="75"/>
       <c r="W106" s="86"/>
       <c r="Y106" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD106" s="19" t="s">
         <v>103</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="111" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B111" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="T117" s="4"/>
       <c r="U117" s="83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V117" s="79"/>
       <c r="W117" s="69"/>
@@ -6502,11 +6502,11 @@
         <v>439401001</v>
       </c>
       <c r="U118" s="83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V118" s="79"/>
       <c r="W118" s="70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X118" s="3"/>
       <c r="Z118" s="3"/>
@@ -6528,12 +6528,12 @@
         <v>1</v>
       </c>
       <c r="T119" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U119" s="32"/>
       <c r="V119" s="76"/>
       <c r="W119" s="70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X119" s="3"/>
       <c r="Z119" s="3"/>
@@ -6571,7 +6571,7 @@
       <c r="U120" s="83"/>
       <c r="V120" s="79"/>
       <c r="W120" s="70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X120" s="3"/>
       <c r="Z120" s="3"/>
@@ -6587,7 +6587,7 @@
       <c r="E121" s="5"/>
       <c r="F121" s="56"/>
       <c r="G121" s="56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -6604,12 +6604,12 @@
         <v>1</v>
       </c>
       <c r="T121" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U121" s="83"/>
       <c r="V121" s="79"/>
       <c r="W121" s="70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X121" s="3"/>
       <c r="Z121" s="3"/>
@@ -6638,14 +6638,14 @@
       <c r="P122" s="5"/>
       <c r="Q122" s="5"/>
       <c r="R122" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S122" s="5" t="s">
         <v>2</v>
       </c>
       <c r="T122" s="80"/>
       <c r="U122" s="85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V122" s="79"/>
       <c r="W122" s="86"/>
@@ -6809,7 +6809,7 @@
       <c r="P127" s="4"/>
       <c r="Q127" s="4"/>
       <c r="R127" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S127" s="6" t="s">
         <v>1</v>
@@ -6848,11 +6848,11 @@
         <v>56</v>
       </c>
       <c r="U128" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="V128" s="76"/>
       <c r="W128" s="70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X128" s="46"/>
       <c r="Y128" s="112"/>
@@ -6886,29 +6886,29 @@
       </c>
       <c r="U129" s="20"/>
       <c r="V129" s="76" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="W129" s="70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Y129" s="2"/>
       <c r="Z129" s="3" t="s">
-        <v>105</v>
+        <v>346</v>
       </c>
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
       <c r="AC129" s="2"/>
       <c r="AD129" s="62" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
       <c r="AE129" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF129" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG129" s="54" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:33" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -6939,29 +6939,29 @@
         <v>54</v>
       </c>
       <c r="U130" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V130" s="79"/>
       <c r="W130" s="70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X130" s="3"/>
       <c r="Y130" s="2"/>
-      <c r="Z130" s="121" t="s">
-        <v>329</v>
+      <c r="Z130" s="118" t="s">
+        <v>327</v>
       </c>
       <c r="AA130" s="3"/>
       <c r="AB130" s="3"/>
       <c r="AC130" s="3"/>
       <c r="AD130" s="3"/>
       <c r="AE130" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AF130" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG130" s="45" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="131" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -6974,7 +6974,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="4"/>
       <c r="I131" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
@@ -6989,14 +6989,14 @@
         <v>1</v>
       </c>
       <c r="T131" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U131" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V131" s="79"/>
       <c r="W131" s="70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="132" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7020,7 +7020,7 @@
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
       <c r="R132" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S132" s="4" t="s">
         <v>2</v>
@@ -7031,26 +7031,26 @@
         <v>99</v>
       </c>
       <c r="W132" s="69" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X132" s="3"/>
       <c r="Z132" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA132" s="3"/>
       <c r="AB132" s="3"/>
       <c r="AC132" s="3"/>
       <c r="AD132" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE132" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF132" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG132" s="54" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="133" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7062,7 +7062,7 @@
       <c r="F133" s="4"/>
       <c r="G133" s="5"/>
       <c r="H133" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
@@ -7074,7 +7074,7 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S133" s="5" t="s">
         <v>2</v>
@@ -7085,20 +7085,20 @@
       <c r="W133" s="70"/>
       <c r="X133" s="3"/>
       <c r="Z133" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA133" s="3"/>
       <c r="AB133" s="3"/>
       <c r="AC133" s="3"/>
       <c r="AD133" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AE133" s="3"/>
       <c r="AF133" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG133" s="54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7132,7 +7132,7 @@
         <v>101</v>
       </c>
       <c r="V134" s="76" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W134" s="70"/>
       <c r="X134" s="3"/>
@@ -7145,13 +7145,13 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
       <c r="AE134" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF134" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG134" s="54" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:33" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7181,13 +7181,13 @@
         <v>56</v>
       </c>
       <c r="U135" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V135" s="76" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W135" s="70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z135" s="3"/>
       <c r="AA135" s="3" t="s">
@@ -7197,13 +7197,13 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
       <c r="AE135" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF135" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG135" s="54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="1:33" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
@@ -7233,11 +7233,11 @@
         <v>56</v>
       </c>
       <c r="U136" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V136" s="76"/>
       <c r="W136" s="70" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Y136" s="55"/>
       <c r="Z136" s="3"/>
@@ -7248,13 +7248,13 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
       <c r="AE136" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF136" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG136" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="137" spans="1:33" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7267,7 +7267,7 @@
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
       <c r="I137" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J137" s="5"/>
       <c r="L137" s="5"/>
@@ -7277,7 +7277,7 @@
       <c r="P137" s="5"/>
       <c r="Q137" s="5"/>
       <c r="R137" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S137" s="5" t="s">
         <v>2</v>
@@ -7286,29 +7286,29 @@
         <v>56</v>
       </c>
       <c r="U137" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V137" s="79"/>
       <c r="W137" s="70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X137" s="3"/>
       <c r="Y137" s="55"/>
       <c r="Z137" s="3"/>
       <c r="AA137" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB137" s="3"/>
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
       <c r="AE137" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF137" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG137" s="54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="138" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7321,7 +7321,7 @@
       <c r="G138" s="5"/>
       <c r="H138" s="5"/>
       <c r="I138" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L138" s="5"/>
       <c r="M138" s="5"/>
@@ -7337,24 +7337,24 @@
         <v>56</v>
       </c>
       <c r="U138" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="V138" s="76"/>
       <c r="W138" s="70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y138" s="55"/>
       <c r="AA138" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AE138" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF138" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG138" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:33" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
@@ -7367,7 +7367,7 @@
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
       <c r="I139" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
@@ -7389,16 +7389,16 @@
       <c r="W139" s="70"/>
       <c r="Y139" s="55"/>
       <c r="AA139" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AE139" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF139" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG139" s="45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="140" spans="1:33" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -7410,7 +7410,7 @@
       <c r="F140" s="4"/>
       <c r="G140" s="5"/>
       <c r="H140" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
@@ -7429,7 +7429,7 @@
       <c r="U140" s="13"/>
       <c r="V140" s="76"/>
       <c r="W140" s="70" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="Y140" s="55"/>
       <c r="AC140" s="2"/>
@@ -7448,7 +7448,7 @@
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
       <c r="I141" s="80" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J141" s="80"/>
       <c r="K141" s="80"/>
@@ -7463,14 +7463,14 @@
         <v>1</v>
       </c>
       <c r="T141" s="80" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="U141" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V141" s="76"/>
       <c r="W141" s="70" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Y141" s="55"/>
       <c r="AC141" s="2"/>
@@ -7577,15 +7577,15 @@
       <c r="S144" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T144" s="122">
+      <c r="T144" s="119">
         <v>90734009</v>
       </c>
       <c r="U144" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V144" s="76"/>
       <c r="W144" s="70" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="Z144" s="62"/>
       <c r="AA144" s="62"/>
@@ -7621,14 +7621,14 @@
         <v>1</v>
       </c>
       <c r="T145" s="57" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="U145" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V145" s="76"/>
       <c r="W145" s="70" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Y145" s="2"/>
     </row>
@@ -7660,11 +7660,11 @@
         <v>54</v>
       </c>
       <c r="U146" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V146" s="76"/>
       <c r="W146" s="70" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="Y146" s="2"/>
       <c r="Z146" s="2"/>
@@ -7683,7 +7683,7 @@
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
       <c r="K147" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L147" s="2"/>
       <c r="M147" s="2"/>
@@ -7696,14 +7696,14 @@
         <v>1</v>
       </c>
       <c r="T147" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U147" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V147" s="76"/>
       <c r="W147" s="70" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Y147" s="2"/>
       <c r="Z147" s="2"/>
@@ -7731,7 +7731,7 @@
       <c r="P148" s="2"/>
       <c r="Q148" s="2"/>
       <c r="R148" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S148" s="3" t="s">
         <v>1</v>
@@ -7741,10 +7741,10 @@
       </c>
       <c r="U148" s="13"/>
       <c r="V148" s="76" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="W148" s="70" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="Y148" s="2"/>
       <c r="Z148" s="2"/>
@@ -7760,7 +7760,7 @@
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
       <c r="H149" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
@@ -7780,26 +7780,26 @@
         <v>102</v>
       </c>
       <c r="V149" s="76" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="W149" s="70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Z149" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AA149" s="2"/>
       <c r="AB149" s="2"/>
       <c r="AC149" s="2"/>
       <c r="AD149" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AE149" s="2"/>
       <c r="AF149" s="3" t="s">
         <v>4</v>
       </c>
       <c r="AG149" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:33" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7812,7 +7812,7 @@
       <c r="G150" s="2"/>
       <c r="H150" s="5"/>
       <c r="I150" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
@@ -7827,14 +7827,14 @@
         <v>1</v>
       </c>
       <c r="T150" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="U150" s="60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V150" s="76"/>
       <c r="W150" s="70" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7946,26 +7946,26 @@
         <v>80</v>
       </c>
       <c r="V155" s="72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W155" s="70" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Y155" s="3"/>
-      <c r="AA155" s="121" t="s">
-        <v>267</v>
+      <c r="AA155" s="118" t="s">
+        <v>266</v>
       </c>
       <c r="AB155" s="3"/>
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
       <c r="AE155" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF155" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG155" s="54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="156" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -8000,7 +8000,7 @@
       </c>
       <c r="V156" s="78"/>
       <c r="W156" s="70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Y156" s="3"/>
       <c r="Z156" s="33"/>
@@ -8055,7 +8055,7 @@
       <c r="H158" s="6"/>
       <c r="I158" s="5"/>
       <c r="K158" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L158" s="5"/>
       <c r="M158" s="4"/>
@@ -8068,14 +8068,14 @@
         <v>1</v>
       </c>
       <c r="T158" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="U158" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V158" s="78"/>
       <c r="W158" s="70" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>